<commit_message>
Updated missed reference (Fryxell et al 1995)
</commit_message>
<xml_diff>
--- a/literature_database/literature_database.xlsx
+++ b/literature_database/literature_database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/verma/Online_resources/literature_database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1D75443-C67B-FA4A-9EEE-6A132461D371}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72558B5B-0D34-E04B-AD00-73AA23E37D40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2160" yWindow="1300" windowWidth="19800" windowHeight="14580" xr2:uid="{48D1C182-AEF1-824A-AF31-3D6131FB60DC}"/>
+    <workbookView xWindow="2900" yWindow="2180" windowWidth="19800" windowHeight="14580" xr2:uid="{48D1C182-AEF1-824A-AF31-3D6131FB60DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="286">
   <si>
     <t xml:space="preserve">Literature Review of Synthetic Gene Drive Technology </t>
   </si>
@@ -920,12 +920,30 @@
   <si>
     <t>Breakdown - Yes</t>
   </si>
+  <si>
+    <t>Journal of Economic Entomology</t>
+  </si>
+  <si>
+    <t>Fryxell KJ, Miller TA. Autocidal biological control: a general strategy for insect control based on genetic transformation with a highly conserved gene. Journal of Economic Entomology. 1995 Oct 1;88(5):1221-32.</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1093/jee/88.5.1221</t>
+  </si>
+  <si>
+    <t>Experiment</t>
+  </si>
+  <si>
+    <t>Sensitizing</t>
+  </si>
+  <si>
+    <t>"The earliest demonstration of synthetic gene drive (sensitizing drives) was carried out by Fryxell and Miller in 1995 "</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19">
+  <fonts count="20">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1059,6 +1077,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF2A2A2A"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1181,7 +1205,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1400,6 +1424,15 @@
     <xf numFmtId="0" fontId="18" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1878,13 +1911,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>40</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>16</c:v>
@@ -1893,7 +1926,7 @@
                   <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>17</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>24</c:v>
@@ -2402,13 +2435,13 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>11</c:v>
@@ -4086,8 +4119,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E9F55AF-FB3A-6E45-BFC6-20E562A75AFE}">
   <dimension ref="A1:U68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4111,29 +4144,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="24" customHeight="1">
-      <c r="A1" s="81" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
-      <c r="I1" s="82"/>
-      <c r="J1" s="82"/>
-      <c r="K1" s="82"/>
-      <c r="L1" s="82"/>
-      <c r="M1" s="82"/>
-      <c r="N1" s="82"/>
-      <c r="O1" s="82"/>
-      <c r="P1" s="82"/>
-      <c r="Q1" s="82"/>
-      <c r="R1" s="82"/>
-      <c r="S1" s="82"/>
-      <c r="T1" s="82"/>
-      <c r="U1" s="83"/>
+      <c r="A1" s="84" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
+      <c r="I1" s="85"/>
+      <c r="J1" s="85"/>
+      <c r="K1" s="85"/>
+      <c r="L1" s="85"/>
+      <c r="M1" s="85"/>
+      <c r="N1" s="85"/>
+      <c r="O1" s="85"/>
+      <c r="P1" s="85"/>
+      <c r="Q1" s="85"/>
+      <c r="R1" s="85"/>
+      <c r="S1" s="85"/>
+      <c r="T1" s="85"/>
+      <c r="U1" s="86"/>
     </row>
     <row r="2" spans="1:21" s="7" customFormat="1" ht="51">
       <c r="A2" s="5" t="s">
@@ -7085,16 +7118,16 @@
       <c r="C50" s="10" t="s">
         <v>257</v>
       </c>
-      <c r="D50" s="3">
-        <v>1</v>
-      </c>
-      <c r="E50" s="3">
-        <v>1</v>
-      </c>
-      <c r="F50" s="3">
+      <c r="D50" s="18">
+        <v>1</v>
+      </c>
+      <c r="E50" s="18">
+        <v>1</v>
+      </c>
+      <c r="F50" s="18">
         <v>2019</v>
       </c>
-      <c r="G50" s="63" t="s">
+      <c r="G50" s="82" t="s">
         <v>235</v>
       </c>
       <c r="H50" s="35" t="s">
@@ -7138,25 +7171,61 @@
       </c>
       <c r="U50" s="13"/>
     </row>
-    <row r="51" spans="1:21">
-      <c r="A51" s="3"/>
-      <c r="B51" s="11"/>
-      <c r="C51" s="11"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="3"/>
-      <c r="G51" s="17"/>
-      <c r="H51" s="3"/>
-      <c r="I51" s="67"/>
-      <c r="J51" s="3"/>
-      <c r="K51" s="3"/>
-      <c r="L51" s="3"/>
-      <c r="M51" s="3"/>
-      <c r="N51" s="3"/>
-      <c r="O51" s="3"/>
-      <c r="P51" s="3"/>
-      <c r="Q51" s="3"/>
-      <c r="R51" s="13"/>
+    <row r="51" spans="1:21" ht="129" customHeight="1">
+      <c r="A51" s="3">
+        <v>49</v>
+      </c>
+      <c r="B51" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="C51" s="81" t="s">
+        <v>280</v>
+      </c>
+      <c r="D51" s="18">
+        <v>0</v>
+      </c>
+      <c r="E51" s="18">
+        <v>0</v>
+      </c>
+      <c r="F51" s="18">
+        <v>1995</v>
+      </c>
+      <c r="G51" s="82" t="s">
+        <v>281</v>
+      </c>
+      <c r="H51" s="83" t="s">
+        <v>282</v>
+      </c>
+      <c r="I51" s="67">
+        <v>5</v>
+      </c>
+      <c r="J51" s="45" t="s">
+        <v>269</v>
+      </c>
+      <c r="K51" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="L51" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="M51" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N51" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="O51" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="P51" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q51" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="R51" s="13" t="s">
+        <v>285</v>
+      </c>
       <c r="S51" s="13"/>
       <c r="T51" s="13"/>
       <c r="U51" s="13"/>
@@ -7598,6 +7667,7 @@
     <hyperlink ref="H48" r:id="rId38" xr:uid="{0E63125C-3A6E-1F42-B212-272182F8F31E}"/>
     <hyperlink ref="H49" r:id="rId39" xr:uid="{02456DD8-B45F-6B41-9AB9-D17BAA3DC4A7}"/>
     <hyperlink ref="H50" r:id="rId40" xr:uid="{99738256-C76A-1E4A-B128-3B19433EFC8E}"/>
+    <hyperlink ref="H51" r:id="rId41" xr:uid="{9748E7DD-AEBB-8944-9FB7-E2226F944909}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -7608,8 +7678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{178CD172-0D52-754C-82C4-99997D10B8F8}">
   <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -7677,7 +7747,7 @@
       <c r="A2" s="73"/>
       <c r="B2" s="74">
         <f>COUNTIF(Sheet1!B3:B100,"Peer reviewed")</f>
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C2" s="74">
         <f>COUNTIF(Sheet1!E3:E100,1)</f>
@@ -7685,7 +7755,7 @@
       </c>
       <c r="D2" s="74">
         <f>COUNTIF(Sheet1!I3:I101,"&lt;=50")</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" s="74">
         <f>COUNTIF(Sheet1!J3:J100,"*Mosquitoes*")</f>
@@ -7697,7 +7767,7 @@
       </c>
       <c r="G2" s="74">
         <f>COUNTIF(Sheet1!P3:P100,"*Suppression*")+COUNTIF(Sheet1!P3:P100,"*Both*")</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H2" s="74">
         <f>COUNTIF(Sheet1!Q3:Q100,1)</f>
@@ -7734,7 +7804,7 @@
       </c>
       <c r="C3" s="72">
         <f>COUNTIF(Sheet1!E3:E100,0)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D3" s="72">
         <f>COUNTIF(Sheet1!I3:I101,"&gt;=50")</f>
@@ -7742,7 +7812,7 @@
       </c>
       <c r="E3" s="72">
         <f>COUNTIF(Sheet1!J3:J100,"*Fruit Fly*")</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F3" s="72">
         <f>COUNTIF(Sheet1!N3:N100,1)</f>

</xml_diff>

<commit_message>
Added: Mathematical modeling of self-contained CRISPR gene drive reversal systems.
</commit_message>
<xml_diff>
--- a/literature_database/literature_database.xlsx
+++ b/literature_database/literature_database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/verma/Online_resources/literature_database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80122357-DC07-5144-B47B-233CB27E2DFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BE68081-E432-A94D-8E1A-848CC5931F06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11180" yWindow="780" windowWidth="24200" windowHeight="15940" xr2:uid="{48D1C182-AEF1-824A-AF31-3D6131FB60DC}"/>
+    <workbookView xWindow="4600" yWindow="780" windowWidth="24200" windowHeight="15940" xr2:uid="{48D1C182-AEF1-824A-AF31-3D6131FB60DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="312">
   <si>
     <t xml:space="preserve">Literature Review of Synthetic Gene Drive Technology </t>
   </si>
@@ -1006,6 +1006,15 @@
   </si>
   <si>
     <t>Underdominance</t>
+  </si>
+  <si>
+    <t>Heffel MG, Finnigan GC. Mathematical modeling of self-contained CRISPR gene drive reversal systems. Scientific Reports. 2019 Dec 27;9(1):1-0.</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1038/s41598-019-54805-8</t>
+  </si>
+  <si>
+    <t>CRISPR, Homing Endonuclease Genes (HEGs)</t>
   </si>
 </sst>
 </file>
@@ -1281,7 +1290,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1365,9 +1374,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1376,9 +1382,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1471,9 +1474,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1494,20 +1494,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1521,6 +1509,21 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1990,10 +1993,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>47</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>46</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>11</c:v>
@@ -2002,10 +2005,10 @@
                   <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>27</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>23</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>28</c:v>
@@ -2517,7 +2520,7 @@
                   <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>33</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>9</c:v>
@@ -2529,7 +2532,7 @@
                   <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>14</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2738,7 +2741,7 @@
                   <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>18</c:v>
@@ -4198,8 +4201,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E9F55AF-FB3A-6E45-BFC6-20E562A75AFE}">
   <dimension ref="A1:U70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4207,15 +4210,15 @@
     <col min="2" max="3" width="17.5" customWidth="1"/>
     <col min="4" max="6" width="10.83203125" style="16" customWidth="1"/>
     <col min="7" max="8" width="29.6640625" customWidth="1"/>
-    <col min="9" max="9" width="23.5" style="63" customWidth="1"/>
+    <col min="9" max="9" width="23.5" style="61" customWidth="1"/>
     <col min="10" max="10" width="16.6640625" customWidth="1"/>
-    <col min="11" max="11" width="17" customWidth="1"/>
-    <col min="12" max="12" width="16.1640625" customWidth="1"/>
-    <col min="13" max="13" width="13.1640625" customWidth="1"/>
-    <col min="14" max="14" width="11.83203125" customWidth="1"/>
-    <col min="15" max="15" width="11" customWidth="1"/>
-    <col min="16" max="16" width="19.33203125" customWidth="1"/>
-    <col min="17" max="17" width="18.33203125" style="65" customWidth="1"/>
+    <col min="11" max="11" width="17" style="2" customWidth="1"/>
+    <col min="12" max="12" width="16.1640625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="13.1640625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="11.83203125" style="2" customWidth="1"/>
+    <col min="15" max="15" width="11" style="16" customWidth="1"/>
+    <col min="16" max="16" width="19.33203125" style="16" customWidth="1"/>
+    <col min="17" max="17" width="18.33203125" style="16" customWidth="1"/>
     <col min="18" max="18" width="32.33203125" customWidth="1"/>
     <col min="19" max="19" width="31.83203125" customWidth="1"/>
     <col min="20" max="20" width="27.6640625" customWidth="1"/>
@@ -4223,29 +4226,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="24" customHeight="1">
-      <c r="A1" s="78" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
-      <c r="J1" s="79"/>
-      <c r="K1" s="79"/>
-      <c r="L1" s="79"/>
-      <c r="M1" s="79"/>
-      <c r="N1" s="79"/>
-      <c r="O1" s="79"/>
-      <c r="P1" s="79"/>
-      <c r="Q1" s="79"/>
-      <c r="R1" s="79"/>
-      <c r="S1" s="79"/>
-      <c r="T1" s="79"/>
-      <c r="U1" s="80"/>
+      <c r="A1" s="81" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
+      <c r="I1" s="82"/>
+      <c r="J1" s="82"/>
+      <c r="K1" s="82"/>
+      <c r="L1" s="82"/>
+      <c r="M1" s="82"/>
+      <c r="N1" s="82"/>
+      <c r="O1" s="82"/>
+      <c r="P1" s="82"/>
+      <c r="Q1" s="82"/>
+      <c r="R1" s="82"/>
+      <c r="S1" s="82"/>
+      <c r="T1" s="82"/>
+      <c r="U1" s="83"/>
     </row>
     <row r="2" spans="1:21" s="7" customFormat="1" ht="51">
       <c r="A2" s="5" t="s">
@@ -4272,7 +4275,7 @@
       <c r="H2" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="I2" s="61" t="s">
+      <c r="I2" s="59" t="s">
         <v>12</v>
       </c>
       <c r="J2" s="6" t="s">
@@ -4293,7 +4296,7 @@
       <c r="O2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="P2" s="5" t="s">
         <v>10</v>
       </c>
       <c r="Q2" s="5" t="s">
@@ -4325,19 +4328,19 @@
       <c r="D3" s="10" t="s">
         <v>185</v>
       </c>
-      <c r="E3" s="35">
-        <v>1</v>
-      </c>
-      <c r="F3" s="35">
+      <c r="E3" s="33">
+        <v>1</v>
+      </c>
+      <c r="F3" s="33">
         <v>2017</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="H3" s="30" t="s">
+      <c r="H3" s="29" t="s">
         <v>158</v>
       </c>
-      <c r="I3" s="60">
+      <c r="I3" s="58">
         <v>70</v>
       </c>
       <c r="J3" s="10" t="s">
@@ -4358,7 +4361,7 @@
       <c r="O3" s="3">
         <v>1</v>
       </c>
-      <c r="P3" s="4" t="s">
+      <c r="P3" s="10" t="s">
         <v>270</v>
       </c>
       <c r="Q3" s="10">
@@ -4403,7 +4406,7 @@
       <c r="H4" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="I4" s="62">
+      <c r="I4" s="60">
         <v>100</v>
       </c>
       <c r="J4" s="3" t="s">
@@ -4424,7 +4427,7 @@
       <c r="O4" s="3">
         <v>1</v>
       </c>
-      <c r="P4" s="11" t="s">
+      <c r="P4" s="3" t="s">
         <v>22</v>
       </c>
       <c r="Q4" s="10">
@@ -4463,7 +4466,7 @@
       <c r="H5" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="I5" s="62">
+      <c r="I5" s="60">
         <v>100</v>
       </c>
       <c r="J5" s="3" t="s">
@@ -4484,7 +4487,7 @@
       <c r="O5" s="3">
         <v>0</v>
       </c>
-      <c r="P5" s="12" t="s">
+      <c r="P5" s="10" t="s">
         <v>270</v>
       </c>
       <c r="Q5" s="10">
@@ -4513,10 +4516,10 @@
       <c r="D6" s="10" t="s">
         <v>185</v>
       </c>
-      <c r="E6" s="36">
-        <v>1</v>
-      </c>
-      <c r="F6" s="36">
+      <c r="E6" s="34">
+        <v>1</v>
+      </c>
+      <c r="F6" s="34">
         <v>2019</v>
       </c>
       <c r="G6" s="20" t="s">
@@ -4525,7 +4528,7 @@
       <c r="H6" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="I6" s="62" t="s">
+      <c r="I6" s="60" t="s">
         <v>39</v>
       </c>
       <c r="J6" s="3" t="s">
@@ -4546,7 +4549,7 @@
       <c r="O6" s="3">
         <v>0</v>
       </c>
-      <c r="P6" s="29" t="s">
+      <c r="P6" s="85" t="s">
         <v>39</v>
       </c>
       <c r="Q6" s="3" t="s">
@@ -4591,7 +4594,7 @@
       <c r="H7" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="I7" s="62">
+      <c r="I7" s="60">
         <v>10</v>
       </c>
       <c r="J7" s="3" t="s">
@@ -4612,7 +4615,7 @@
       <c r="O7" s="3">
         <v>0</v>
       </c>
-      <c r="P7" s="11" t="s">
+      <c r="P7" s="3" t="s">
         <v>36</v>
       </c>
       <c r="Q7" s="10">
@@ -4653,7 +4656,7 @@
       <c r="H8" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="I8" s="62" t="s">
+      <c r="I8" s="60" t="s">
         <v>39</v>
       </c>
       <c r="J8" s="10" t="s">
@@ -4674,7 +4677,7 @@
       <c r="O8" s="3">
         <v>0</v>
       </c>
-      <c r="P8" s="12" t="s">
+      <c r="P8" s="10" t="s">
         <v>48</v>
       </c>
       <c r="Q8" s="3" t="s">
@@ -4701,7 +4704,7 @@
       <c r="B9" s="12" t="s">
         <v>253</v>
       </c>
-      <c r="C9" s="39" t="s">
+      <c r="C9" s="37" t="s">
         <v>244</v>
       </c>
       <c r="D9" s="25">
@@ -4719,7 +4722,7 @@
       <c r="H9" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="I9" s="62" t="s">
+      <c r="I9" s="60" t="s">
         <v>54</v>
       </c>
       <c r="J9" s="3" t="s">
@@ -4740,7 +4743,7 @@
       <c r="O9" s="3">
         <v>0</v>
       </c>
-      <c r="P9" s="1"/>
+      <c r="P9" s="3"/>
       <c r="Q9" s="10">
         <v>1</v>
       </c>
@@ -4773,16 +4776,16 @@
       <c r="F10" s="3">
         <v>2018</v>
       </c>
-      <c r="G10" s="48" t="s">
+      <c r="G10" s="46" t="s">
         <v>60</v>
       </c>
       <c r="H10" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="I10" s="62">
+      <c r="I10" s="60">
         <v>10</v>
       </c>
-      <c r="J10" s="40" t="s">
+      <c r="J10" s="38" t="s">
         <v>268</v>
       </c>
       <c r="K10" s="11" t="s">
@@ -4800,7 +4803,7 @@
       <c r="O10" s="3">
         <v>0</v>
       </c>
-      <c r="P10" s="12" t="s">
+      <c r="P10" s="10" t="s">
         <v>62</v>
       </c>
       <c r="Q10" s="3">
@@ -4841,7 +4844,7 @@
       <c r="H11" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="I11" s="62">
+      <c r="I11" s="60">
         <v>100</v>
       </c>
       <c r="J11" s="3" t="s">
@@ -4896,13 +4899,13 @@
       <c r="F12" s="3">
         <v>2014</v>
       </c>
-      <c r="G12" s="48" t="s">
+      <c r="G12" s="46" t="s">
         <v>70</v>
       </c>
       <c r="H12" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="I12" s="62" t="s">
+      <c r="I12" s="60" t="s">
         <v>39</v>
       </c>
       <c r="J12" s="28" t="s">
@@ -4923,7 +4926,7 @@
       <c r="O12" s="3">
         <v>0</v>
       </c>
-      <c r="P12" s="29" t="s">
+      <c r="P12" s="85" t="s">
         <v>39</v>
       </c>
       <c r="Q12" s="3">
@@ -4959,10 +4962,10 @@
       <c r="G13" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="H13" s="30" t="s">
+      <c r="H13" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="I13" s="62" t="s">
+      <c r="I13" s="60" t="s">
         <v>39</v>
       </c>
       <c r="J13" s="3" t="s">
@@ -4983,7 +4986,7 @@
       <c r="O13" s="3">
         <v>0</v>
       </c>
-      <c r="P13" s="29" t="s">
+      <c r="P13" s="85" t="s">
         <v>39</v>
       </c>
       <c r="Q13" s="3">
@@ -5018,13 +5021,13 @@
       <c r="F14" s="3">
         <v>2017</v>
       </c>
-      <c r="G14" s="48" t="s">
+      <c r="G14" s="46" t="s">
         <v>79</v>
       </c>
-      <c r="H14" s="30" t="s">
+      <c r="H14" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="I14" s="60">
+      <c r="I14" s="58">
         <v>90</v>
       </c>
       <c r="J14" s="3" t="s">
@@ -5045,7 +5048,7 @@
       <c r="O14" s="3">
         <v>1</v>
       </c>
-      <c r="P14" s="11" t="s">
+      <c r="P14" s="3" t="s">
         <v>54</v>
       </c>
       <c r="Q14" s="3">
@@ -5058,7 +5061,7 @@
       <c r="T14" s="13"/>
       <c r="U14" s="13"/>
     </row>
-    <row r="15" spans="1:21" ht="112">
+    <row r="15" spans="1:21" ht="128">
       <c r="A15" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -5078,16 +5081,16 @@
       <c r="F15" s="10">
         <v>2013</v>
       </c>
-      <c r="G15" s="48" t="s">
+      <c r="G15" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="H15" s="30" t="s">
+      <c r="H15" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="I15" s="62">
+      <c r="I15" s="60">
         <v>30</v>
       </c>
-      <c r="J15" s="40" t="s">
+      <c r="J15" s="38" t="s">
         <v>268</v>
       </c>
       <c r="K15" s="12" t="s">
@@ -5105,7 +5108,7 @@
       <c r="O15" s="3">
         <v>1</v>
       </c>
-      <c r="P15" s="4" t="s">
+      <c r="P15" s="10" t="s">
         <v>270</v>
       </c>
       <c r="Q15" s="3">
@@ -5142,13 +5145,13 @@
       <c r="F16" s="3">
         <v>2011</v>
       </c>
-      <c r="G16" s="48" t="s">
+      <c r="G16" s="46" t="s">
         <v>188</v>
       </c>
-      <c r="H16" s="30" t="s">
+      <c r="H16" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="I16" s="62">
+      <c r="I16" s="60">
         <v>80</v>
       </c>
       <c r="J16" s="5" t="s">
@@ -5169,7 +5172,7 @@
       <c r="O16" s="3">
         <v>1</v>
       </c>
-      <c r="P16" s="11"/>
+      <c r="P16" s="3"/>
       <c r="Q16" s="3">
         <v>0</v>
       </c>
@@ -5202,19 +5205,19 @@
       <c r="F17" s="3">
         <v>2007</v>
       </c>
-      <c r="G17" s="32" t="s">
+      <c r="G17" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="H17" s="30" t="s">
+      <c r="H17" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="I17" s="62">
+      <c r="I17" s="60">
         <v>80</v>
       </c>
       <c r="J17" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="K17" s="31" t="s">
+      <c r="K17" s="30" t="s">
         <v>169</v>
       </c>
       <c r="L17" s="3" t="s">
@@ -5229,7 +5232,7 @@
       <c r="O17" s="3">
         <v>0</v>
       </c>
-      <c r="P17" s="11" t="s">
+      <c r="P17" s="3" t="s">
         <v>97</v>
       </c>
       <c r="Q17" s="3">
@@ -5267,10 +5270,10 @@
       <c r="G18" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="H18" s="30" t="s">
+      <c r="H18" s="29" t="s">
         <v>101</v>
       </c>
-      <c r="I18" s="62">
+      <c r="I18" s="60">
         <v>70</v>
       </c>
       <c r="J18" s="5" t="s">
@@ -5291,7 +5294,7 @@
       <c r="O18" s="3">
         <v>0</v>
       </c>
-      <c r="P18" s="33" t="s">
+      <c r="P18" s="38" t="s">
         <v>36</v>
       </c>
       <c r="Q18" s="10">
@@ -5329,10 +5332,10 @@
       <c r="G19" s="17" t="s">
         <v>186</v>
       </c>
-      <c r="H19" s="30" t="s">
+      <c r="H19" s="29" t="s">
         <v>103</v>
       </c>
-      <c r="I19" s="62">
+      <c r="I19" s="60">
         <v>70</v>
       </c>
       <c r="J19" s="3" t="s">
@@ -5353,7 +5356,7 @@
       <c r="O19" s="3">
         <v>1</v>
       </c>
-      <c r="P19" s="11" t="s">
+      <c r="P19" s="3" t="s">
         <v>97</v>
       </c>
       <c r="Q19" s="3">
@@ -5391,16 +5394,16 @@
       <c r="G20" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="H20" s="30" t="s">
+      <c r="H20" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="I20" s="62">
+      <c r="I20" s="60">
         <v>90</v>
       </c>
       <c r="J20" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="K20" s="34" t="s">
+      <c r="K20" s="32" t="s">
         <v>108</v>
       </c>
       <c r="L20" s="3" t="s">
@@ -5415,7 +5418,7 @@
       <c r="O20" s="3">
         <v>0</v>
       </c>
-      <c r="P20" s="12" t="s">
+      <c r="P20" s="10" t="s">
         <v>270</v>
       </c>
       <c r="Q20" s="3">
@@ -5454,7 +5457,7 @@
       <c r="H21" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="I21" s="62">
+      <c r="I21" s="60">
         <v>40</v>
       </c>
       <c r="J21" s="3" t="s">
@@ -5475,7 +5478,7 @@
       <c r="O21" s="3">
         <v>0</v>
       </c>
-      <c r="P21" s="12" t="s">
+      <c r="P21" s="10" t="s">
         <v>270</v>
       </c>
       <c r="Q21" s="3"/>
@@ -5511,10 +5514,10 @@
       <c r="G22" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="H22" s="42" t="s">
+      <c r="H22" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="I22" s="62">
+      <c r="I22" s="60">
         <v>70</v>
       </c>
       <c r="J22" s="3" t="s">
@@ -5535,7 +5538,7 @@
       <c r="O22" s="3">
         <v>0</v>
       </c>
-      <c r="P22" s="11" t="s">
+      <c r="P22" s="3" t="s">
         <v>97</v>
       </c>
       <c r="Q22" s="10">
@@ -5574,7 +5577,7 @@
       <c r="H23" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="I23" s="62">
+      <c r="I23" s="60">
         <v>90</v>
       </c>
       <c r="J23" s="3" t="s">
@@ -5595,7 +5598,7 @@
       <c r="O23" s="3">
         <v>0</v>
       </c>
-      <c r="P23" s="11"/>
+      <c r="P23" s="3"/>
       <c r="Q23" s="3">
         <v>1</v>
       </c>
@@ -5631,10 +5634,10 @@
       <c r="G24" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="H24" s="30" t="s">
+      <c r="H24" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="I24" s="62">
+      <c r="I24" s="60">
         <v>80</v>
       </c>
       <c r="J24" s="3" t="s">
@@ -5655,7 +5658,7 @@
       <c r="O24" s="3">
         <v>1</v>
       </c>
-      <c r="P24" s="11" t="s">
+      <c r="P24" s="3" t="s">
         <v>36</v>
       </c>
       <c r="Q24" s="3">
@@ -5693,13 +5696,13 @@
       <c r="G25" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="H25" s="30" t="s">
+      <c r="H25" s="29" t="s">
         <v>127</v>
       </c>
-      <c r="I25" s="62">
+      <c r="I25" s="60">
         <v>30</v>
       </c>
-      <c r="J25" s="40" t="s">
+      <c r="J25" s="38" t="s">
         <v>268</v>
       </c>
       <c r="K25" s="11" t="s">
@@ -5717,7 +5720,7 @@
       <c r="O25" s="3">
         <v>0</v>
       </c>
-      <c r="P25" s="11"/>
+      <c r="P25" s="3"/>
       <c r="Q25" s="3">
         <v>1</v>
       </c>
@@ -5755,13 +5758,13 @@
       <c r="G26" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="H26" s="30" t="s">
+      <c r="H26" s="29" t="s">
         <v>132</v>
       </c>
-      <c r="I26" s="62">
+      <c r="I26" s="60">
         <v>30</v>
       </c>
-      <c r="J26" s="40" t="s">
+      <c r="J26" s="38" t="s">
         <v>268</v>
       </c>
       <c r="K26" s="11" t="s">
@@ -5779,7 +5782,7 @@
       <c r="O26" s="3">
         <v>0</v>
       </c>
-      <c r="P26" s="11" t="s">
+      <c r="P26" s="3" t="s">
         <v>97</v>
       </c>
       <c r="Q26" s="3">
@@ -5815,10 +5818,10 @@
       <c r="G27" s="17" t="s">
         <v>135</v>
       </c>
-      <c r="H27" s="30" t="s">
+      <c r="H27" s="29" t="s">
         <v>134</v>
       </c>
-      <c r="I27" s="62">
+      <c r="I27" s="60">
         <v>90</v>
       </c>
       <c r="J27" s="5" t="s">
@@ -5839,7 +5842,7 @@
       <c r="O27" s="3">
         <v>1</v>
       </c>
-      <c r="P27" s="11"/>
+      <c r="P27" s="3"/>
       <c r="Q27" s="3">
         <v>0</v>
       </c>
@@ -5875,10 +5878,10 @@
       <c r="G28" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="H28" s="30" t="s">
+      <c r="H28" s="29" t="s">
         <v>140</v>
       </c>
-      <c r="I28" s="62">
+      <c r="I28" s="60">
         <v>90</v>
       </c>
       <c r="J28" s="3" t="s">
@@ -5899,7 +5902,7 @@
       <c r="O28" s="3">
         <v>0</v>
       </c>
-      <c r="P28" s="11" t="s">
+      <c r="P28" s="3" t="s">
         <v>97</v>
       </c>
       <c r="Q28" s="3">
@@ -5932,19 +5935,19 @@
       <c r="F29" s="3">
         <v>2016</v>
       </c>
-      <c r="G29" s="37" t="s">
+      <c r="G29" s="35" t="s">
         <v>142</v>
       </c>
       <c r="H29" s="21" t="s">
         <v>143</v>
       </c>
-      <c r="I29" s="62">
+      <c r="I29" s="60">
         <v>90</v>
       </c>
       <c r="J29" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="K29" s="64" t="s">
+      <c r="K29" s="62" t="s">
         <v>162</v>
       </c>
       <c r="L29" s="10" t="s">
@@ -5959,7 +5962,7 @@
       <c r="O29" s="3">
         <v>0</v>
       </c>
-      <c r="P29" s="11" t="s">
+      <c r="P29" s="3" t="s">
         <v>19</v>
       </c>
       <c r="Q29" s="3" t="s">
@@ -5995,16 +5998,16 @@
       <c r="G30" s="17" t="s">
         <v>160</v>
       </c>
-      <c r="H30" s="30" t="s">
+      <c r="H30" s="29" t="s">
         <v>144</v>
       </c>
-      <c r="I30" s="62">
+      <c r="I30" s="60">
         <v>90</v>
       </c>
       <c r="J30" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="K30" s="43" t="s">
+      <c r="K30" s="41" t="s">
         <v>161</v>
       </c>
       <c r="L30" s="10" t="s">
@@ -6019,7 +6022,7 @@
       <c r="O30" s="3">
         <v>1</v>
       </c>
-      <c r="P30" s="12" t="s">
+      <c r="P30" s="10" t="s">
         <v>270</v>
       </c>
       <c r="Q30" s="3">
@@ -6041,10 +6044,10 @@
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="B31" s="39" t="s">
+      <c r="B31" s="37" t="s">
         <v>253</v>
       </c>
-      <c r="C31" s="39" t="s">
+      <c r="C31" s="37" t="s">
         <v>260</v>
       </c>
       <c r="D31" s="25">
@@ -6059,10 +6062,10 @@
       <c r="G31" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="H31" s="30" t="s">
+      <c r="H31" s="29" t="s">
         <v>146</v>
       </c>
-      <c r="I31" s="62" t="s">
+      <c r="I31" s="60" t="s">
         <v>54</v>
       </c>
       <c r="J31" s="3" t="s">
@@ -6083,7 +6086,7 @@
       <c r="O31" s="3">
         <v>0</v>
       </c>
-      <c r="P31" s="11" t="s">
+      <c r="P31" s="3" t="s">
         <v>19</v>
       </c>
       <c r="Q31" s="3" t="s">
@@ -6118,16 +6121,16 @@
       <c r="F32" s="3">
         <v>2018</v>
       </c>
-      <c r="G32" s="38" t="s">
+      <c r="G32" s="36" t="s">
         <v>187</v>
       </c>
-      <c r="H32" s="30" t="s">
+      <c r="H32" s="29" t="s">
         <v>147</v>
       </c>
-      <c r="I32" s="62">
+      <c r="I32" s="60">
         <v>60</v>
       </c>
-      <c r="J32" s="40" t="s">
+      <c r="J32" s="38" t="s">
         <v>268</v>
       </c>
       <c r="K32" s="11" t="s">
@@ -6181,10 +6184,10 @@
       <c r="G33" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="H33" s="40" t="s">
+      <c r="H33" s="38" t="s">
         <v>148</v>
       </c>
-      <c r="I33" s="60">
+      <c r="I33" s="58">
         <v>80</v>
       </c>
       <c r="J33" s="5" t="s">
@@ -6245,16 +6248,16 @@
       <c r="G34" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="H34" s="30" t="s">
+      <c r="H34" s="29" t="s">
         <v>151</v>
       </c>
-      <c r="I34" s="62">
+      <c r="I34" s="60">
         <v>90</v>
       </c>
       <c r="J34" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="K34" s="45" t="s">
+      <c r="K34" s="43" t="s">
         <v>177</v>
       </c>
       <c r="L34" s="3" t="s">
@@ -6269,13 +6272,13 @@
       <c r="O34" s="3">
         <v>0</v>
       </c>
-      <c r="P34" s="46" t="s">
+      <c r="P34" s="44" t="s">
         <v>36</v>
       </c>
       <c r="Q34" s="3">
         <v>0</v>
       </c>
-      <c r="R34" s="44" t="s">
+      <c r="R34" s="42" t="s">
         <v>176</v>
       </c>
       <c r="S34" s="13"/>
@@ -6305,16 +6308,16 @@
       <c r="G35" s="17" t="s">
         <v>153</v>
       </c>
-      <c r="H35" s="41" t="s">
+      <c r="H35" s="39" t="s">
         <v>152</v>
       </c>
-      <c r="I35" s="62">
+      <c r="I35" s="60">
         <v>100</v>
       </c>
       <c r="J35" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="K35" s="47" t="s">
+      <c r="K35" s="45" t="s">
         <v>177</v>
       </c>
       <c r="L35" s="3" t="s">
@@ -6365,10 +6368,10 @@
       <c r="G36" s="17" t="s">
         <v>157</v>
       </c>
-      <c r="H36" s="30" t="s">
+      <c r="H36" s="29" t="s">
         <v>154</v>
       </c>
-      <c r="I36" s="62">
+      <c r="I36" s="60">
         <v>90</v>
       </c>
       <c r="J36" s="3" t="s">
@@ -6427,16 +6430,16 @@
       <c r="G37" s="17" t="s">
         <v>156</v>
       </c>
-      <c r="H37" s="30" t="s">
+      <c r="H37" s="29" t="s">
         <v>155</v>
       </c>
-      <c r="I37" s="62">
+      <c r="I37" s="60">
         <v>70</v>
       </c>
       <c r="J37" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="K37" s="45" t="s">
+      <c r="K37" s="43" t="s">
         <v>181</v>
       </c>
       <c r="L37" s="3" t="s">
@@ -6482,10 +6485,10 @@
       <c r="F38" s="3">
         <v>2016</v>
       </c>
-      <c r="G38" s="51" t="s">
+      <c r="G38" s="49" t="s">
         <v>193</v>
       </c>
-      <c r="H38" s="30" t="s">
+      <c r="H38" s="29" t="s">
         <v>196</v>
       </c>
       <c r="I38" s="3" t="s">
@@ -6537,7 +6540,7 @@
       <c r="E39" s="3">
         <v>1</v>
       </c>
-      <c r="F39" s="49">
+      <c r="F39" s="47">
         <v>2018</v>
       </c>
       <c r="G39" s="13" t="s">
@@ -6598,7 +6601,7 @@
       <c r="F40" s="3">
         <v>2017</v>
       </c>
-      <c r="G40" s="50" t="s">
+      <c r="G40" s="48" t="s">
         <v>194</v>
       </c>
       <c r="H40" s="3" t="s">
@@ -6714,13 +6717,13 @@
       <c r="F42" s="3">
         <v>2017</v>
       </c>
-      <c r="G42" s="56" t="s">
+      <c r="G42" s="54" t="s">
         <v>199</v>
       </c>
-      <c r="H42" s="54" t="s">
+      <c r="H42" s="52" t="s">
         <v>200</v>
       </c>
-      <c r="I42" s="60">
+      <c r="I42" s="58">
         <v>50</v>
       </c>
       <c r="J42" s="7" t="s">
@@ -6747,7 +6750,7 @@
       <c r="Q42" s="10">
         <v>1</v>
       </c>
-      <c r="R42" s="52" t="s">
+      <c r="R42" s="50" t="s">
         <v>202</v>
       </c>
       <c r="S42" s="13" t="s">
@@ -6776,13 +6779,13 @@
       <c r="F43" s="3">
         <v>2017</v>
       </c>
-      <c r="G43" s="55" t="s">
+      <c r="G43" s="53" t="s">
         <v>204</v>
       </c>
-      <c r="H43" s="30" t="s">
+      <c r="H43" s="29" t="s">
         <v>205</v>
       </c>
-      <c r="I43" s="62">
+      <c r="I43" s="60">
         <v>100</v>
       </c>
       <c r="J43" s="3" t="s">
@@ -6836,13 +6839,13 @@
       <c r="F44" s="3">
         <v>2019</v>
       </c>
-      <c r="G44" s="56" t="s">
+      <c r="G44" s="54" t="s">
         <v>207</v>
       </c>
-      <c r="H44" s="53" t="s">
+      <c r="H44" s="51" t="s">
         <v>208</v>
       </c>
-      <c r="I44" s="62">
+      <c r="I44" s="60">
         <v>100</v>
       </c>
       <c r="J44" s="10" t="s">
@@ -6896,13 +6899,13 @@
       <c r="F45" s="3">
         <v>2018</v>
       </c>
-      <c r="G45" s="56" t="s">
+      <c r="G45" s="54" t="s">
         <v>212</v>
       </c>
       <c r="H45" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I45" s="62">
+      <c r="I45" s="60">
         <v>100</v>
       </c>
       <c r="J45" s="3" t="s">
@@ -6958,13 +6961,13 @@
       <c r="F46" s="3">
         <v>2019</v>
       </c>
-      <c r="G46" s="56" t="s">
+      <c r="G46" s="54" t="s">
         <v>216</v>
       </c>
       <c r="H46" s="21" t="s">
         <v>217</v>
       </c>
-      <c r="I46" s="62">
+      <c r="I46" s="60">
         <v>100</v>
       </c>
       <c r="J46" s="10" t="s">
@@ -7020,13 +7023,13 @@
       <c r="F47" s="3">
         <v>2014</v>
       </c>
-      <c r="G47" s="58" t="s">
+      <c r="G47" s="56" t="s">
         <v>220</v>
       </c>
-      <c r="H47" s="30" t="s">
+      <c r="H47" s="29" t="s">
         <v>221</v>
       </c>
-      <c r="I47" s="62">
+      <c r="I47" s="60">
         <v>80</v>
       </c>
       <c r="J47" s="5" t="s">
@@ -7053,7 +7056,7 @@
       <c r="Q47" s="3">
         <v>0</v>
       </c>
-      <c r="R47" s="57" t="s">
+      <c r="R47" s="55" t="s">
         <v>223</v>
       </c>
       <c r="S47" s="13" t="s">
@@ -7086,16 +7089,16 @@
       <c r="F48" s="3">
         <v>2015</v>
       </c>
-      <c r="G48" s="55" t="s">
+      <c r="G48" s="53" t="s">
         <v>227</v>
       </c>
-      <c r="H48" s="59" t="s">
+      <c r="H48" s="57" t="s">
         <v>228</v>
       </c>
-      <c r="I48" s="62">
+      <c r="I48" s="60">
         <v>5</v>
       </c>
-      <c r="J48" s="40" t="s">
+      <c r="J48" s="38" t="s">
         <v>268</v>
       </c>
       <c r="K48" s="3" t="s">
@@ -7147,10 +7150,10 @@
       <c r="G49" s="17" t="s">
         <v>230</v>
       </c>
-      <c r="H49" s="30" t="s">
+      <c r="H49" s="29" t="s">
         <v>231</v>
       </c>
-      <c r="I49" s="62" t="s">
+      <c r="I49" s="60" t="s">
         <v>39</v>
       </c>
       <c r="J49" s="3" t="s">
@@ -7206,13 +7209,13 @@
       <c r="F50" s="18">
         <v>2019</v>
       </c>
-      <c r="G50" s="76" t="s">
+      <c r="G50" s="73" t="s">
         <v>234</v>
       </c>
-      <c r="H50" s="30" t="s">
+      <c r="H50" s="29" t="s">
         <v>235</v>
       </c>
-      <c r="I50" s="62">
+      <c r="I50" s="60">
         <v>5</v>
       </c>
       <c r="J50" s="3" t="s">
@@ -7257,7 +7260,7 @@
       <c r="B51" s="10" t="s">
         <v>253</v>
       </c>
-      <c r="C51" s="75" t="s">
+      <c r="C51" s="72" t="s">
         <v>279</v>
       </c>
       <c r="D51" s="18">
@@ -7269,16 +7272,16 @@
       <c r="F51" s="18">
         <v>1995</v>
       </c>
-      <c r="G51" s="84" t="s">
+      <c r="G51" s="77" t="s">
         <v>280</v>
       </c>
-      <c r="H51" s="77" t="s">
+      <c r="H51" s="74" t="s">
         <v>281</v>
       </c>
-      <c r="I51" s="62">
+      <c r="I51" s="60">
         <v>5</v>
       </c>
-      <c r="J51" s="40" t="s">
+      <c r="J51" s="38" t="s">
         <v>268</v>
       </c>
       <c r="K51" s="3" t="s">
@@ -7328,19 +7331,19 @@
       <c r="F52" s="3">
         <v>2019</v>
       </c>
-      <c r="G52" s="85" t="s">
+      <c r="G52" s="78" t="s">
         <v>285</v>
       </c>
-      <c r="H52" s="30" t="s">
+      <c r="H52" s="29" t="s">
         <v>286</v>
       </c>
-      <c r="I52" s="62">
+      <c r="I52" s="60">
         <v>90</v>
       </c>
       <c r="J52" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="K52" s="86" t="s">
+      <c r="K52" s="79" t="s">
         <v>288</v>
       </c>
       <c r="L52" s="3"/>
@@ -7383,13 +7386,13 @@
       <c r="F53" s="3">
         <v>2019</v>
       </c>
-      <c r="G53" s="87" t="s">
+      <c r="G53" s="80" t="s">
         <v>289</v>
       </c>
-      <c r="H53" s="30" t="s">
+      <c r="H53" s="29" t="s">
         <v>291</v>
       </c>
-      <c r="I53" s="62" t="s">
+      <c r="I53" s="60" t="s">
         <v>292</v>
       </c>
       <c r="J53" s="3" t="s">
@@ -7443,10 +7446,10 @@
       <c r="G54" s="17" t="s">
         <v>295</v>
       </c>
-      <c r="H54" s="53" t="s">
+      <c r="H54" s="51" t="s">
         <v>293</v>
       </c>
-      <c r="I54" s="62">
+      <c r="I54" s="60">
         <v>80</v>
       </c>
       <c r="J54" s="3" t="s">
@@ -7500,10 +7503,10 @@
       <c r="G55" s="17" t="s">
         <v>297</v>
       </c>
-      <c r="H55" s="77" t="s">
+      <c r="H55" s="74" t="s">
         <v>298</v>
       </c>
-      <c r="I55" s="62">
+      <c r="I55" s="60">
         <v>20</v>
       </c>
       <c r="J55" s="3" t="s">
@@ -7557,10 +7560,10 @@
       <c r="G56" s="17" t="s">
         <v>300</v>
       </c>
-      <c r="H56" s="30" t="s">
+      <c r="H56" s="29" t="s">
         <v>302</v>
       </c>
-      <c r="I56" s="62">
+      <c r="I56" s="60">
         <v>80</v>
       </c>
       <c r="J56" s="3" t="s">
@@ -7614,10 +7617,10 @@
       <c r="G57" s="17" t="s">
         <v>306</v>
       </c>
-      <c r="H57" s="77" t="s">
+      <c r="H57" s="74" t="s">
         <v>305</v>
       </c>
-      <c r="I57" s="62">
+      <c r="I57" s="60">
         <v>80</v>
       </c>
       <c r="J57" s="3" t="s">
@@ -7649,24 +7652,58 @@
       <c r="T57" s="13"/>
       <c r="U57" s="13"/>
     </row>
-    <row r="58" spans="1:21" ht="115" customHeight="1">
-      <c r="A58" s="3"/>
-      <c r="B58" s="3"/>
-      <c r="C58" s="3"/>
-      <c r="D58" s="3"/>
-      <c r="E58" s="3"/>
-      <c r="F58" s="3"/>
-      <c r="G58" s="1"/>
-      <c r="H58" s="81"/>
-      <c r="I58" s="62"/>
-      <c r="J58" s="1"/>
-      <c r="K58" s="1"/>
-      <c r="L58" s="1"/>
-      <c r="M58" s="82"/>
-      <c r="N58" s="82"/>
-      <c r="O58" s="82"/>
-      <c r="P58" s="1"/>
-      <c r="Q58" s="82"/>
+    <row r="58" spans="1:21" ht="107" customHeight="1">
+      <c r="A58" s="3">
+        <v>56</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="D58" s="3">
+        <v>1</v>
+      </c>
+      <c r="E58" s="3">
+        <v>1</v>
+      </c>
+      <c r="F58" s="3">
+        <v>2019</v>
+      </c>
+      <c r="G58" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="H58" s="74" t="s">
+        <v>310</v>
+      </c>
+      <c r="I58" s="60">
+        <v>90</v>
+      </c>
+      <c r="J58" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="K58" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="L58" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="M58" s="3">
+        <v>1</v>
+      </c>
+      <c r="N58" s="3">
+        <v>0</v>
+      </c>
+      <c r="O58" s="3">
+        <v>0</v>
+      </c>
+      <c r="P58" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q58" s="3">
+        <v>0</v>
+      </c>
       <c r="R58" s="13"/>
       <c r="S58" s="13"/>
       <c r="T58" s="13"/>
@@ -7680,16 +7717,16 @@
       <c r="E59" s="3"/>
       <c r="F59" s="3"/>
       <c r="G59" s="1"/>
-      <c r="H59" s="81"/>
-      <c r="I59" s="62"/>
+      <c r="H59" s="75"/>
+      <c r="I59" s="60"/>
       <c r="J59" s="1"/>
-      <c r="K59" s="1"/>
-      <c r="L59" s="1"/>
-      <c r="M59" s="82"/>
-      <c r="N59" s="82"/>
-      <c r="O59" s="82"/>
-      <c r="P59" s="1"/>
-      <c r="Q59" s="82"/>
+      <c r="K59" s="84"/>
+      <c r="L59" s="84"/>
+      <c r="M59" s="3"/>
+      <c r="N59" s="3"/>
+      <c r="O59" s="3"/>
+      <c r="P59" s="3"/>
+      <c r="Q59" s="3"/>
       <c r="R59" s="13"/>
       <c r="S59" s="13"/>
       <c r="T59" s="13"/>
@@ -7703,16 +7740,16 @@
       <c r="E60" s="3"/>
       <c r="F60" s="3"/>
       <c r="G60" s="1"/>
-      <c r="H60" s="81"/>
-      <c r="I60" s="62"/>
+      <c r="H60" s="75"/>
+      <c r="I60" s="60"/>
       <c r="J60" s="1"/>
-      <c r="K60" s="1"/>
-      <c r="L60" s="1"/>
-      <c r="M60" s="82"/>
-      <c r="N60" s="82"/>
-      <c r="O60" s="82"/>
-      <c r="P60" s="1"/>
-      <c r="Q60" s="82"/>
+      <c r="K60" s="84"/>
+      <c r="L60" s="84"/>
+      <c r="M60" s="3"/>
+      <c r="N60" s="3"/>
+      <c r="O60" s="3"/>
+      <c r="P60" s="3"/>
+      <c r="Q60" s="3"/>
       <c r="R60" s="13"/>
       <c r="S60" s="13"/>
       <c r="T60" s="13"/>
@@ -7726,16 +7763,16 @@
       <c r="E61" s="3"/>
       <c r="F61" s="3"/>
       <c r="G61" s="1"/>
-      <c r="H61" s="81"/>
-      <c r="I61" s="62"/>
+      <c r="H61" s="75"/>
+      <c r="I61" s="60"/>
       <c r="J61" s="1"/>
-      <c r="K61" s="1"/>
-      <c r="L61" s="1"/>
-      <c r="M61" s="82"/>
-      <c r="N61" s="82"/>
-      <c r="O61" s="82"/>
-      <c r="P61" s="1"/>
-      <c r="Q61" s="82"/>
+      <c r="K61" s="84"/>
+      <c r="L61" s="84"/>
+      <c r="M61" s="3"/>
+      <c r="N61" s="3"/>
+      <c r="O61" s="3"/>
+      <c r="P61" s="3"/>
+      <c r="Q61" s="3"/>
       <c r="R61" s="13"/>
       <c r="S61" s="13"/>
       <c r="T61" s="13"/>
@@ -7749,16 +7786,16 @@
       <c r="E62" s="3"/>
       <c r="F62" s="3"/>
       <c r="G62" s="1"/>
-      <c r="H62" s="81"/>
-      <c r="I62" s="62"/>
+      <c r="H62" s="75"/>
+      <c r="I62" s="60"/>
       <c r="J62" s="1"/>
-      <c r="K62" s="1"/>
-      <c r="L62" s="1"/>
-      <c r="M62" s="82"/>
-      <c r="N62" s="82"/>
-      <c r="O62" s="82"/>
-      <c r="P62" s="1"/>
-      <c r="Q62" s="82"/>
+      <c r="K62" s="84"/>
+      <c r="L62" s="84"/>
+      <c r="M62" s="3"/>
+      <c r="N62" s="3"/>
+      <c r="O62" s="3"/>
+      <c r="P62" s="3"/>
+      <c r="Q62" s="3"/>
       <c r="R62" s="13"/>
       <c r="S62" s="13"/>
       <c r="T62" s="13"/>
@@ -7772,16 +7809,16 @@
       <c r="E63" s="3"/>
       <c r="F63" s="3"/>
       <c r="G63" s="1"/>
-      <c r="H63" s="81"/>
-      <c r="I63" s="62"/>
+      <c r="H63" s="75"/>
+      <c r="I63" s="60"/>
       <c r="J63" s="1"/>
-      <c r="K63" s="1"/>
-      <c r="L63" s="1"/>
-      <c r="M63" s="82"/>
-      <c r="N63" s="82"/>
-      <c r="O63" s="82"/>
-      <c r="P63" s="1"/>
-      <c r="Q63" s="82"/>
+      <c r="K63" s="84"/>
+      <c r="L63" s="84"/>
+      <c r="M63" s="3"/>
+      <c r="N63" s="3"/>
+      <c r="O63" s="3"/>
+      <c r="P63" s="3"/>
+      <c r="Q63" s="3"/>
       <c r="R63" s="13"/>
       <c r="S63" s="13"/>
       <c r="T63" s="13"/>
@@ -7795,16 +7832,16 @@
       <c r="E64" s="3"/>
       <c r="F64" s="3"/>
       <c r="G64" s="1"/>
-      <c r="H64" s="81"/>
-      <c r="I64" s="62"/>
+      <c r="H64" s="75"/>
+      <c r="I64" s="60"/>
       <c r="J64" s="1"/>
-      <c r="K64" s="1"/>
-      <c r="L64" s="1"/>
-      <c r="M64" s="82"/>
-      <c r="N64" s="82"/>
-      <c r="O64" s="82"/>
-      <c r="P64" s="1"/>
-      <c r="Q64" s="82"/>
+      <c r="K64" s="84"/>
+      <c r="L64" s="84"/>
+      <c r="M64" s="3"/>
+      <c r="N64" s="3"/>
+      <c r="O64" s="3"/>
+      <c r="P64" s="3"/>
+      <c r="Q64" s="3"/>
       <c r="R64" s="13"/>
       <c r="S64" s="13"/>
       <c r="T64" s="13"/>
@@ -7818,16 +7855,16 @@
       <c r="E65" s="3"/>
       <c r="F65" s="3"/>
       <c r="G65" s="1"/>
-      <c r="H65" s="81"/>
-      <c r="I65" s="62"/>
+      <c r="H65" s="75"/>
+      <c r="I65" s="60"/>
       <c r="J65" s="1"/>
-      <c r="K65" s="1"/>
-      <c r="L65" s="1"/>
-      <c r="M65" s="82"/>
-      <c r="N65" s="82"/>
-      <c r="O65" s="82"/>
-      <c r="P65" s="1"/>
-      <c r="Q65" s="82"/>
+      <c r="K65" s="84"/>
+      <c r="L65" s="84"/>
+      <c r="M65" s="3"/>
+      <c r="N65" s="3"/>
+      <c r="O65" s="3"/>
+      <c r="P65" s="3"/>
+      <c r="Q65" s="3"/>
       <c r="R65" s="13"/>
       <c r="S65" s="13"/>
       <c r="T65" s="13"/>
@@ -7841,16 +7878,16 @@
       <c r="E66" s="3"/>
       <c r="F66" s="3"/>
       <c r="G66" s="1"/>
-      <c r="H66" s="81"/>
-      <c r="I66" s="62"/>
+      <c r="H66" s="75"/>
+      <c r="I66" s="60"/>
       <c r="J66" s="1"/>
-      <c r="K66" s="1"/>
-      <c r="L66" s="1"/>
-      <c r="M66" s="82"/>
-      <c r="N66" s="82"/>
-      <c r="O66" s="82"/>
-      <c r="P66" s="1"/>
-      <c r="Q66" s="82"/>
+      <c r="K66" s="84"/>
+      <c r="L66" s="84"/>
+      <c r="M66" s="3"/>
+      <c r="N66" s="3"/>
+      <c r="O66" s="3"/>
+      <c r="P66" s="3"/>
+      <c r="Q66" s="3"/>
       <c r="R66" s="13"/>
       <c r="S66" s="13"/>
       <c r="T66" s="13"/>
@@ -7864,16 +7901,16 @@
       <c r="E67" s="3"/>
       <c r="F67" s="3"/>
       <c r="G67" s="1"/>
-      <c r="H67" s="81"/>
-      <c r="I67" s="62"/>
+      <c r="H67" s="75"/>
+      <c r="I67" s="60"/>
       <c r="J67" s="1"/>
-      <c r="K67" s="1"/>
-      <c r="L67" s="1"/>
-      <c r="M67" s="82"/>
-      <c r="N67" s="82"/>
-      <c r="O67" s="82"/>
-      <c r="P67" s="1"/>
-      <c r="Q67" s="82"/>
+      <c r="K67" s="84"/>
+      <c r="L67" s="84"/>
+      <c r="M67" s="3"/>
+      <c r="N67" s="3"/>
+      <c r="O67" s="3"/>
+      <c r="P67" s="3"/>
+      <c r="Q67" s="3"/>
       <c r="R67" s="13"/>
       <c r="S67" s="13"/>
       <c r="T67" s="13"/>
@@ -7887,16 +7924,16 @@
       <c r="E68" s="3"/>
       <c r="F68" s="3"/>
       <c r="G68" s="1"/>
-      <c r="H68" s="81"/>
-      <c r="I68" s="62"/>
+      <c r="H68" s="75"/>
+      <c r="I68" s="60"/>
       <c r="J68" s="1"/>
-      <c r="K68" s="1"/>
-      <c r="L68" s="1"/>
-      <c r="M68" s="82"/>
-      <c r="N68" s="82"/>
-      <c r="O68" s="82"/>
-      <c r="P68" s="1"/>
-      <c r="Q68" s="82"/>
+      <c r="K68" s="84"/>
+      <c r="L68" s="84"/>
+      <c r="M68" s="3"/>
+      <c r="N68" s="3"/>
+      <c r="O68" s="3"/>
+      <c r="P68" s="3"/>
+      <c r="Q68" s="3"/>
       <c r="R68" s="13"/>
       <c r="S68" s="13"/>
       <c r="T68" s="13"/>
@@ -7911,15 +7948,15 @@
       <c r="F69" s="3"/>
       <c r="G69" s="1"/>
       <c r="H69" s="1"/>
-      <c r="I69" s="83"/>
+      <c r="I69" s="76"/>
       <c r="J69" s="1"/>
-      <c r="K69" s="1"/>
-      <c r="L69" s="1"/>
-      <c r="M69" s="1"/>
-      <c r="N69" s="1"/>
-      <c r="O69" s="1"/>
-      <c r="P69" s="1"/>
-      <c r="Q69" s="82"/>
+      <c r="K69" s="84"/>
+      <c r="L69" s="84"/>
+      <c r="M69" s="84"/>
+      <c r="N69" s="84"/>
+      <c r="O69" s="3"/>
+      <c r="P69" s="3"/>
+      <c r="Q69" s="3"/>
       <c r="R69" s="1"/>
       <c r="S69" s="1"/>
       <c r="T69" s="1"/>
@@ -7934,15 +7971,15 @@
       <c r="F70" s="3"/>
       <c r="G70" s="1"/>
       <c r="H70" s="1"/>
-      <c r="I70" s="83"/>
+      <c r="I70" s="76"/>
       <c r="J70" s="1"/>
-      <c r="K70" s="1"/>
-      <c r="L70" s="1"/>
-      <c r="M70" s="1"/>
-      <c r="N70" s="1"/>
-      <c r="O70" s="1"/>
-      <c r="P70" s="1"/>
-      <c r="Q70" s="82"/>
+      <c r="K70" s="84"/>
+      <c r="L70" s="84"/>
+      <c r="M70" s="84"/>
+      <c r="N70" s="84"/>
+      <c r="O70" s="3"/>
+      <c r="P70" s="3"/>
+      <c r="Q70" s="3"/>
       <c r="R70" s="1"/>
       <c r="S70" s="1"/>
       <c r="T70" s="1"/>
@@ -8001,6 +8038,7 @@
     <hyperlink ref="H55" r:id="rId45" xr:uid="{D02C6F54-81ED-8A4A-9FC2-AA25B415331F}"/>
     <hyperlink ref="H56" r:id="rId46" xr:uid="{3F243643-47F8-9642-BBB1-C073EA51E282}"/>
     <hyperlink ref="H57" r:id="rId47" xr:uid="{88D9FA4D-9F9C-5F42-B1D2-EA4F848C4896}"/>
+    <hyperlink ref="H58" r:id="rId48" xr:uid="{78C03330-D5C3-AB42-A027-FB4049D534AF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -8027,221 +8065,221 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="64" t="s">
         <v>271</v>
       </c>
-      <c r="B1" s="73">
-        <v>1</v>
-      </c>
-      <c r="C1" s="73">
+      <c r="B1" s="70">
+        <v>1</v>
+      </c>
+      <c r="C1" s="70">
         <v>2</v>
       </c>
-      <c r="D1" s="73">
+      <c r="D1" s="70">
         <v>3</v>
       </c>
-      <c r="E1" s="73">
+      <c r="E1" s="70">
         <v>4</v>
       </c>
-      <c r="F1" s="73">
+      <c r="F1" s="70">
         <v>5</v>
       </c>
-      <c r="G1" s="73">
+      <c r="G1" s="70">
         <v>6</v>
       </c>
-      <c r="H1" s="73">
+      <c r="H1" s="70">
         <v>7</v>
       </c>
-      <c r="J1" s="67" t="s">
+      <c r="J1" s="64" t="s">
         <v>271</v>
       </c>
-      <c r="K1" s="73">
-        <v>1</v>
-      </c>
-      <c r="L1" s="74">
+      <c r="K1" s="70">
+        <v>1</v>
+      </c>
+      <c r="L1" s="71">
         <v>2</v>
       </c>
-      <c r="M1" s="74">
+      <c r="M1" s="71">
         <v>3</v>
       </c>
-      <c r="N1" s="73">
+      <c r="N1" s="70">
         <v>4</v>
       </c>
-      <c r="O1" s="73">
+      <c r="O1" s="70">
         <v>5</v>
       </c>
-      <c r="P1" s="73">
+      <c r="P1" s="70">
         <v>6</v>
       </c>
-      <c r="Q1" s="73">
+      <c r="Q1" s="70">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:17">
-      <c r="A2" s="67"/>
-      <c r="B2" s="68">
+      <c r="A2" s="64"/>
+      <c r="B2" s="65">
         <f>COUNTIF(Sheet1!B3:B100,"Peer reviewed")</f>
+        <v>48</v>
+      </c>
+      <c r="C2" s="65">
+        <f>COUNTIF(Sheet1!E3:E100,1)</f>
         <v>47</v>
       </c>
-      <c r="C2" s="68">
-        <f>COUNTIF(Sheet1!E3:E100,1)</f>
-        <v>46</v>
-      </c>
-      <c r="D2" s="68">
+      <c r="D2" s="65">
         <f>COUNTIF(Sheet1!I3:I101,"&lt;=50")</f>
         <v>11</v>
       </c>
-      <c r="E2" s="68">
+      <c r="E2" s="65">
         <f>COUNTIF(Sheet1!J3:J100,"*Mosquitoes*")</f>
         <v>17</v>
       </c>
-      <c r="F2" s="68">
+      <c r="F2" s="65">
         <f>COUNTIF(Sheet1!M3:M100,1)</f>
-        <v>27</v>
-      </c>
-      <c r="G2" s="68">
+        <v>28</v>
+      </c>
+      <c r="G2" s="65">
         <f>COUNTIF(Sheet1!P3:P100,"*Suppression*")+COUNTIF(Sheet1!P3:P100,"*Both*")</f>
-        <v>23</v>
-      </c>
-      <c r="H2" s="68">
+        <v>24</v>
+      </c>
+      <c r="H2" s="65">
         <f>COUNTIF(Sheet1!Q3:Q100,1)</f>
         <v>28</v>
       </c>
-      <c r="J2" s="70"/>
-      <c r="K2" s="68" t="s">
+      <c r="J2" s="67"/>
+      <c r="K2" s="65" t="s">
         <v>253</v>
       </c>
-      <c r="L2" s="68" t="s">
+      <c r="L2" s="65" t="s">
         <v>272</v>
       </c>
-      <c r="M2" s="68" t="s">
+      <c r="M2" s="65" t="s">
         <v>273</v>
       </c>
-      <c r="N2" s="68" t="s">
+      <c r="N2" s="65" t="s">
         <v>55</v>
       </c>
-      <c r="O2" s="68" t="s">
+      <c r="O2" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="P2" s="68" t="s">
+      <c r="P2" s="65" t="s">
         <v>277</v>
       </c>
-      <c r="Q2" s="68" t="s">
+      <c r="Q2" s="65" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="3" spans="1:17">
-      <c r="A3" s="67"/>
-      <c r="B3" s="66">
+      <c r="A3" s="64"/>
+      <c r="B3" s="63">
         <f>COUNTIF(Sheet1!B3:B100,"Report")</f>
         <v>4</v>
       </c>
-      <c r="C3" s="66">
+      <c r="C3" s="63">
         <f>COUNTIF(Sheet1!E3:E100,0)</f>
         <v>9</v>
       </c>
-      <c r="D3" s="66">
+      <c r="D3" s="63">
         <f>COUNTIF(Sheet1!I3:I101,"&gt;=50")</f>
-        <v>33</v>
-      </c>
-      <c r="E3" s="66">
+        <v>34</v>
+      </c>
+      <c r="E3" s="63">
         <f>COUNTIF(Sheet1!J3:J100,"*Fruit Fly*")</f>
         <v>9</v>
       </c>
-      <c r="F3" s="66">
+      <c r="F3" s="63">
         <f>COUNTIF(Sheet1!N3:N100,1)</f>
         <v>14</v>
       </c>
-      <c r="G3" s="66">
+      <c r="G3" s="63">
         <f>COUNTIF(Sheet1!P3:P100,"*Replacement*")+COUNTIF(Sheet1!P3:P100,"*Both*")</f>
         <v>21</v>
       </c>
-      <c r="H3" s="66">
+      <c r="H3" s="63">
         <f>COUNTIF(Sheet1!Q3:Q100,0)</f>
-        <v>14</v>
-      </c>
-      <c r="J3" s="70"/>
-      <c r="K3" s="71" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="67"/>
+      <c r="K3" s="68" t="s">
         <v>191</v>
       </c>
-      <c r="L3" s="71" t="s">
+      <c r="L3" s="68" t="s">
         <v>197</v>
       </c>
-      <c r="M3" s="71" t="s">
+      <c r="M3" s="68" t="s">
         <v>274</v>
       </c>
-      <c r="N3" s="71" t="s">
+      <c r="N3" s="68" t="s">
         <v>198</v>
       </c>
-      <c r="O3" s="71" t="s">
+      <c r="O3" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="P3" s="71" t="s">
+      <c r="P3" s="68" t="s">
         <v>97</v>
       </c>
-      <c r="Q3" s="71" t="s">
+      <c r="Q3" s="68" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:17">
-      <c r="A4" s="67"/>
-      <c r="B4" s="68">
+      <c r="A4" s="64"/>
+      <c r="B4" s="65">
         <f>COUNTIF(Sheet1!B3:B100,"Preprint")</f>
         <v>4</v>
       </c>
-      <c r="C4" s="68"/>
-      <c r="D4" s="69">
+      <c r="C4" s="65"/>
+      <c r="D4" s="66">
         <f>COUNTIF(Sheet1!I3:I100,"Perspective")+COUNTIF(Sheet1!I3:I100,"Report")+COUNTIF(Sheet1!I3:I100,"Review")</f>
         <v>12</v>
       </c>
-      <c r="E4" s="68">
+      <c r="E4" s="65">
         <f>COUNTIF(Sheet1!J3:J100,"*Generic*")</f>
-        <v>16</v>
-      </c>
-      <c r="F4" s="68">
+        <v>17</v>
+      </c>
+      <c r="F4" s="65">
         <f>COUNTIF(Sheet1!O3:O100,1)</f>
         <v>18</v>
       </c>
-      <c r="G4" s="68"/>
-      <c r="H4" s="68"/>
-      <c r="J4" s="70"/>
-      <c r="K4" s="68" t="s">
+      <c r="G4" s="65"/>
+      <c r="H4" s="65"/>
+      <c r="J4" s="67"/>
+      <c r="K4" s="65" t="s">
         <v>255</v>
       </c>
-      <c r="L4" s="68"/>
-      <c r="M4" s="72" t="s">
+      <c r="L4" s="65"/>
+      <c r="M4" s="69" t="s">
         <v>275</v>
       </c>
-      <c r="N4" s="68" t="s">
+      <c r="N4" s="65" t="s">
         <v>66</v>
       </c>
-      <c r="O4" s="68" t="s">
+      <c r="O4" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="68"/>
-      <c r="Q4" s="68"/>
+      <c r="P4" s="65"/>
+      <c r="Q4" s="65"/>
     </row>
     <row r="5" spans="1:17">
-      <c r="A5" s="67"/>
-      <c r="B5" s="66"/>
-      <c r="C5" s="66"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66">
+      <c r="A5" s="64"/>
+      <c r="B5" s="63"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63">
         <f>COUNTIF(Sheet1!J3:J100,"*Rodents*")+COUNTIF(Sheet1!J4:J101,"*Beetle*")</f>
         <v>3</v>
       </c>
-      <c r="F5" s="66"/>
-      <c r="G5" s="66"/>
-      <c r="H5" s="66"/>
-      <c r="J5" s="70"/>
-      <c r="K5" s="71"/>
-      <c r="L5" s="71"/>
-      <c r="M5" s="71"/>
-      <c r="N5" s="71" t="s">
+      <c r="F5" s="63"/>
+      <c r="G5" s="63"/>
+      <c r="H5" s="63"/>
+      <c r="J5" s="67"/>
+      <c r="K5" s="68"/>
+      <c r="L5" s="68"/>
+      <c r="M5" s="68"/>
+      <c r="N5" s="68" t="s">
         <v>276</v>
       </c>
-      <c r="O5" s="71"/>
-      <c r="P5" s="71"/>
-      <c r="Q5" s="71"/>
+      <c r="O5" s="68"/>
+      <c r="P5" s="68"/>
+      <c r="Q5" s="68"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Gene drive and resilience through renewal with next generation Cleave and Rescue selfish genetic elements
</commit_message>
<xml_diff>
--- a/literature_database/literature_database.xlsx
+++ b/literature_database/literature_database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/verma/Online_resources/literature_database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BE68081-E432-A94D-8E1A-848CC5931F06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{089B3388-AC4C-7143-ADB7-E06BAF6B7721}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4600" yWindow="780" windowWidth="24200" windowHeight="15940" xr2:uid="{48D1C182-AEF1-824A-AF31-3D6131FB60DC}"/>
+    <workbookView xWindow="460" yWindow="780" windowWidth="24200" windowHeight="15940" xr2:uid="{48D1C182-AEF1-824A-AF31-3D6131FB60DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="314">
   <si>
     <t xml:space="preserve">Literature Review of Synthetic Gene Drive Technology </t>
   </si>
@@ -1015,6 +1015,12 @@
   </si>
   <si>
     <t>CRISPR, Homing Endonuclease Genes (HEGs)</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1073/pnas.1921698117</t>
+  </si>
+  <si>
+    <t>Cleave and Rescue, CRIPR</t>
   </si>
 </sst>
 </file>
@@ -1290,7 +1296,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1510,6 +1516,12 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1519,11 +1531,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1993,13 +2002,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>48</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>47</c:v>
-                </c:pt>
                 <c:pt idx="2">
-                  <c:v>11</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>17</c:v>
@@ -2011,7 +2020,7 @@
                   <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>28</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2523,13 +2532,13 @@
                   <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>21</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>15</c:v>
@@ -4201,8 +4210,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E9F55AF-FB3A-6E45-BFC6-20E562A75AFE}">
   <dimension ref="A1:U70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="R59" sqref="R59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4226,29 +4235,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="24" customHeight="1">
-      <c r="A1" s="81" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
-      <c r="I1" s="82"/>
-      <c r="J1" s="82"/>
-      <c r="K1" s="82"/>
-      <c r="L1" s="82"/>
-      <c r="M1" s="82"/>
-      <c r="N1" s="82"/>
-      <c r="O1" s="82"/>
-      <c r="P1" s="82"/>
-      <c r="Q1" s="82"/>
-      <c r="R1" s="82"/>
-      <c r="S1" s="82"/>
-      <c r="T1" s="82"/>
-      <c r="U1" s="83"/>
+      <c r="A1" s="83" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="84"/>
+      <c r="L1" s="84"/>
+      <c r="M1" s="84"/>
+      <c r="N1" s="84"/>
+      <c r="O1" s="84"/>
+      <c r="P1" s="84"/>
+      <c r="Q1" s="84"/>
+      <c r="R1" s="84"/>
+      <c r="S1" s="84"/>
+      <c r="T1" s="84"/>
+      <c r="U1" s="85"/>
     </row>
     <row r="2" spans="1:21" s="7" customFormat="1" ht="51">
       <c r="A2" s="5" t="s">
@@ -4549,7 +4558,7 @@
       <c r="O6" s="3">
         <v>0</v>
       </c>
-      <c r="P6" s="85" t="s">
+      <c r="P6" s="82" t="s">
         <v>39</v>
       </c>
       <c r="Q6" s="3" t="s">
@@ -4926,7 +4935,7 @@
       <c r="O12" s="3">
         <v>0</v>
       </c>
-      <c r="P12" s="85" t="s">
+      <c r="P12" s="82" t="s">
         <v>39</v>
       </c>
       <c r="Q12" s="3">
@@ -4986,7 +4995,7 @@
       <c r="O13" s="3">
         <v>0</v>
       </c>
-      <c r="P13" s="85" t="s">
+      <c r="P13" s="82" t="s">
         <v>39</v>
       </c>
       <c r="Q13" s="3">
@@ -5061,7 +5070,7 @@
       <c r="T14" s="13"/>
       <c r="U14" s="13"/>
     </row>
-    <row r="15" spans="1:21" ht="128">
+    <row r="15" spans="1:21" ht="112">
       <c r="A15" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -7671,7 +7680,7 @@
       <c r="F58" s="3">
         <v>2019</v>
       </c>
-      <c r="G58" s="14" t="s">
+      <c r="G58" s="86" t="s">
         <v>309</v>
       </c>
       <c r="H58" s="74" t="s">
@@ -7710,23 +7719,55 @@
       <c r="U58" s="13"/>
     </row>
     <row r="59" spans="1:21" ht="102" customHeight="1">
-      <c r="A59" s="3"/>
-      <c r="B59" s="3"/>
-      <c r="C59" s="3"/>
-      <c r="D59" s="3"/>
-      <c r="E59" s="3"/>
-      <c r="F59" s="3"/>
+      <c r="A59" s="3">
+        <v>57</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E59" s="3">
+        <v>1</v>
+      </c>
+      <c r="F59" s="3">
+        <v>2020</v>
+      </c>
       <c r="G59" s="1"/>
-      <c r="H59" s="75"/>
-      <c r="I59" s="60"/>
-      <c r="J59" s="1"/>
-      <c r="K59" s="84"/>
-      <c r="L59" s="84"/>
-      <c r="M59" s="3"/>
-      <c r="N59" s="3"/>
-      <c r="O59" s="3"/>
-      <c r="P59" s="3"/>
-      <c r="Q59" s="3"/>
+      <c r="H59" s="29" t="s">
+        <v>312</v>
+      </c>
+      <c r="I59" s="60">
+        <v>10</v>
+      </c>
+      <c r="J59" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="K59" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="L59" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="M59" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N59" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="O59" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="P59" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q59" s="3">
+        <v>1</v>
+      </c>
       <c r="R59" s="13"/>
       <c r="S59" s="13"/>
       <c r="T59" s="13"/>
@@ -7743,8 +7784,8 @@
       <c r="H60" s="75"/>
       <c r="I60" s="60"/>
       <c r="J60" s="1"/>
-      <c r="K60" s="84"/>
-      <c r="L60" s="84"/>
+      <c r="K60" s="81"/>
+      <c r="L60" s="81"/>
       <c r="M60" s="3"/>
       <c r="N60" s="3"/>
       <c r="O60" s="3"/>
@@ -7766,8 +7807,8 @@
       <c r="H61" s="75"/>
       <c r="I61" s="60"/>
       <c r="J61" s="1"/>
-      <c r="K61" s="84"/>
-      <c r="L61" s="84"/>
+      <c r="K61" s="81"/>
+      <c r="L61" s="81"/>
       <c r="M61" s="3"/>
       <c r="N61" s="3"/>
       <c r="O61" s="3"/>
@@ -7789,8 +7830,8 @@
       <c r="H62" s="75"/>
       <c r="I62" s="60"/>
       <c r="J62" s="1"/>
-      <c r="K62" s="84"/>
-      <c r="L62" s="84"/>
+      <c r="K62" s="81"/>
+      <c r="L62" s="81"/>
       <c r="M62" s="3"/>
       <c r="N62" s="3"/>
       <c r="O62" s="3"/>
@@ -7812,8 +7853,8 @@
       <c r="H63" s="75"/>
       <c r="I63" s="60"/>
       <c r="J63" s="1"/>
-      <c r="K63" s="84"/>
-      <c r="L63" s="84"/>
+      <c r="K63" s="81"/>
+      <c r="L63" s="81"/>
       <c r="M63" s="3"/>
       <c r="N63" s="3"/>
       <c r="O63" s="3"/>
@@ -7835,8 +7876,8 @@
       <c r="H64" s="75"/>
       <c r="I64" s="60"/>
       <c r="J64" s="1"/>
-      <c r="K64" s="84"/>
-      <c r="L64" s="84"/>
+      <c r="K64" s="81"/>
+      <c r="L64" s="81"/>
       <c r="M64" s="3"/>
       <c r="N64" s="3"/>
       <c r="O64" s="3"/>
@@ -7858,8 +7899,8 @@
       <c r="H65" s="75"/>
       <c r="I65" s="60"/>
       <c r="J65" s="1"/>
-      <c r="K65" s="84"/>
-      <c r="L65" s="84"/>
+      <c r="K65" s="81"/>
+      <c r="L65" s="81"/>
       <c r="M65" s="3"/>
       <c r="N65" s="3"/>
       <c r="O65" s="3"/>
@@ -7881,8 +7922,8 @@
       <c r="H66" s="75"/>
       <c r="I66" s="60"/>
       <c r="J66" s="1"/>
-      <c r="K66" s="84"/>
-      <c r="L66" s="84"/>
+      <c r="K66" s="81"/>
+      <c r="L66" s="81"/>
       <c r="M66" s="3"/>
       <c r="N66" s="3"/>
       <c r="O66" s="3"/>
@@ -7904,8 +7945,8 @@
       <c r="H67" s="75"/>
       <c r="I67" s="60"/>
       <c r="J67" s="1"/>
-      <c r="K67" s="84"/>
-      <c r="L67" s="84"/>
+      <c r="K67" s="81"/>
+      <c r="L67" s="81"/>
       <c r="M67" s="3"/>
       <c r="N67" s="3"/>
       <c r="O67" s="3"/>
@@ -7927,8 +7968,8 @@
       <c r="H68" s="75"/>
       <c r="I68" s="60"/>
       <c r="J68" s="1"/>
-      <c r="K68" s="84"/>
-      <c r="L68" s="84"/>
+      <c r="K68" s="81"/>
+      <c r="L68" s="81"/>
       <c r="M68" s="3"/>
       <c r="N68" s="3"/>
       <c r="O68" s="3"/>
@@ -7950,10 +7991,10 @@
       <c r="H69" s="1"/>
       <c r="I69" s="76"/>
       <c r="J69" s="1"/>
-      <c r="K69" s="84"/>
-      <c r="L69" s="84"/>
-      <c r="M69" s="84"/>
-      <c r="N69" s="84"/>
+      <c r="K69" s="81"/>
+      <c r="L69" s="81"/>
+      <c r="M69" s="81"/>
+      <c r="N69" s="81"/>
       <c r="O69" s="3"/>
       <c r="P69" s="3"/>
       <c r="Q69" s="3"/>
@@ -7973,10 +8014,10 @@
       <c r="H70" s="1"/>
       <c r="I70" s="76"/>
       <c r="J70" s="1"/>
-      <c r="K70" s="84"/>
-      <c r="L70" s="84"/>
-      <c r="M70" s="84"/>
-      <c r="N70" s="84"/>
+      <c r="K70" s="81"/>
+      <c r="L70" s="81"/>
+      <c r="M70" s="81"/>
+      <c r="N70" s="81"/>
       <c r="O70" s="3"/>
       <c r="P70" s="3"/>
       <c r="Q70" s="3"/>
@@ -8039,6 +8080,7 @@
     <hyperlink ref="H56" r:id="rId46" xr:uid="{3F243643-47F8-9642-BBB1-C073EA51E282}"/>
     <hyperlink ref="H57" r:id="rId47" xr:uid="{88D9FA4D-9F9C-5F42-B1D2-EA4F848C4896}"/>
     <hyperlink ref="H58" r:id="rId48" xr:uid="{78C03330-D5C3-AB42-A027-FB4049D534AF}"/>
+    <hyperlink ref="H59" r:id="rId49" xr:uid="{4C3A9D7B-D77A-0541-BA20-29C30C7D28C6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -8118,15 +8160,15 @@
       <c r="A2" s="64"/>
       <c r="B2" s="65">
         <f>COUNTIF(Sheet1!B3:B100,"Peer reviewed")</f>
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C2" s="65">
         <f>COUNTIF(Sheet1!E3:E100,1)</f>
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D2" s="65">
         <f>COUNTIF(Sheet1!I3:I101,"&lt;=50")</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E2" s="65">
         <f>COUNTIF(Sheet1!J3:J100,"*Mosquitoes*")</f>
@@ -8142,7 +8184,7 @@
       </c>
       <c r="H2" s="65">
         <f>COUNTIF(Sheet1!Q3:Q100,1)</f>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J2" s="67"/>
       <c r="K2" s="65" t="s">
@@ -8183,7 +8225,7 @@
       </c>
       <c r="E3" s="63">
         <f>COUNTIF(Sheet1!J3:J100,"*Fruit Fly*")</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F3" s="63">
         <f>COUNTIF(Sheet1!N3:N100,1)</f>
@@ -8191,7 +8233,7 @@
       </c>
       <c r="G3" s="63">
         <f>COUNTIF(Sheet1!P3:P100,"*Replacement*")+COUNTIF(Sheet1!P3:P100,"*Both*")</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H3" s="63">
         <f>COUNTIF(Sheet1!Q3:Q100,0)</f>

</xml_diff>

<commit_message>
Spelling correction through inbuilt excel spell checker. And some minor corrections such as bioRxiv, arXiv etc.
</commit_message>
<xml_diff>
--- a/literature_database/literature_database.xlsx
+++ b/literature_database/literature_database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/verma/Online_resources/literature_database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B37327C6-8586-F540-BDF7-3CE10AB44E1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17CCB7B5-F1E7-554B-BC64-1C1158A038F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="720" yWindow="900" windowWidth="24200" windowHeight="15940" xr2:uid="{48D1C182-AEF1-824A-AF31-3D6131FB60DC}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="307">
   <si>
     <t xml:space="preserve">Literature Review of Synthetic Gene Drive Technology </t>
   </si>
@@ -64,33 +64,21 @@
     <t>Reference</t>
   </si>
   <si>
-    <t>Aim of the Study (Suppresion/replacement)</t>
-  </si>
-  <si>
     <t>#</t>
   </si>
   <si>
     <t>Scope (Theory/Experiment)</t>
   </si>
   <si>
-    <t xml:space="preserve">how three different gene drive tech- niques—population suppression through dual-germline fertility disruption, population suppression with a driving-Y chromo- some, and population replacement—would fare upon release in two well-studied, field data-rich, and previously modeled settings. </t>
-  </si>
-  <si>
     <t xml:space="preserve">We show that, if an NHEJ allele has wild-type fecundity, it is very difficult for the original gene drive construct to succeed. The population will revert to its preintervention dynamics, but with the original wild type replaced by a resistant genotype. </t>
   </si>
   <si>
-    <t>Epidemological modelling takes into account stochasticity, vector populations, larval dynamics, Adult feeding behaviour, closed egg laying, spatial for human and vectors, migration, data from subsaharan africa</t>
-  </si>
-  <si>
     <t xml:space="preserve">M. R. Vella, C. E. Gunning, A. L. Lloyd, and F. Gould, “Evaluating strategies for reversing CRISPR-Cas9 gene drives,” Scientific Reports, vol. 7, dec 2017. </t>
   </si>
   <si>
     <t xml:space="preserve">C. Noble, B. Adlam, G. M. Church, K. M. Esvelt, and M. A. Nowak, “Current CRISPR gene drive systems are likely to be highly invasive in wild populations,” eLife, vol. 7, June 2018. </t>
   </si>
   <si>
-    <t xml:space="preserve">Emperical data in modelling. Sub Sharan Africa. Namawala (Tanzania) and Garki (Nigeria)  </t>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
@@ -100,18 +88,9 @@
     <t>CRISPR, Homing Endonuclease Genes (HEGs), Driving-Y and Population replacement</t>
   </si>
   <si>
-    <t xml:space="preserve">Studied the effect of realistic seasonality in contrast to non-seasonality on vector population dynamics. Seasonality helps gene drive spread. Explored effect of spatial pattern, release timing, frequency, and migration rate on spread of malaria for 3 gene drive approaches (1) population supression (2) Driving Y (3) Population replacement. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Aim - Stochastic, spatial and migration effect on invasion of drive allele in the population.  </t>
   </si>
   <si>
-    <t>Aim - Analytical modelling to evaluate the efficiency of synthetic resitance, reversal drives and immunizing reversal drives in eliminating HD. Countermeasures against the spread of drive alleles</t>
-  </si>
-  <si>
-    <t>Synthetic resitance and reversal drives are unlikely to prevent Homing drive fixation because of stable polymorphic equlibrium. Immunizing Reversal Drives (IRD) theoretically ensure elimination of HD. But Cas9 remains</t>
-  </si>
-  <si>
     <t>"We conclude with specific recommendations about how to address current challenges and foster more effective communication and decision- making for complex, post-normal issues, such as gene drives."</t>
   </si>
   <si>
@@ -176,32 +155,6 @@
   </si>
   <si>
     <t>Ref 20: "Champer et al. [20] show that resistance to a CRISPR gene drive engineered in the germ line of D. melanogaster"</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve"> Ref 17-19 "Lyttle’s caged popula- tions of </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Drosophila" </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Ref 21: " supported by a new flour beetle study analyzing preexisting DNA sequence variation in genomic sites that would be prime candidates for CRISPR-Cas9 GDSs "</t>
-    </r>
   </si>
   <si>
     <t>Review of different experimental studies leading to resistance in Gene Drive Systems.</t>
@@ -260,9 +213,6 @@
     <t>"we explore the feasibility and effectiveness of gRNA multiplexing, male germline drive activity, and reduction of so- matic activity for resistance reduction by studying several CRISPR homing gene drive constructs in D. melanogaster"</t>
   </si>
   <si>
-    <t>Experiment to demostrate the gRNA multiplexing as mechanism against gene drive resistance.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Use genetic simulation framework SLiM, See Figure 3 </t>
   </si>
   <si>
@@ -275,9 +225,6 @@
     <t>Generic</t>
   </si>
   <si>
-    <t>"Here, we use a population genetics model to compare the expected characteristics of three spatially self-limiting gene drive systems: one-locus underdominance, two-locus underdominance and daisychain drives. We find large differences b"</t>
-  </si>
-  <si>
     <t>Assumptions: Decreate time model, nonoverlapping generations, variable fitness cost for population suppression or replacement, Population is very large, Migration effect taken on 2 island populations, individual mate randomly.</t>
   </si>
   <si>
@@ -302,9 +249,6 @@
     <t>Rodents</t>
   </si>
   <si>
-    <t>Newzealand, gene drive system, risks</t>
-  </si>
-  <si>
     <t>"we explore the risk of accidental spread posed by self-propagating gene drive technologies, highlight new gene drive designs that might achieve better outcomes"</t>
   </si>
   <si>
@@ -335,9 +279,6 @@
     <t>" To investigate the confinement properties of single- and two-locus UDMEL, we follow the framework of Marshall and Hay"</t>
   </si>
   <si>
-    <t xml:space="preserve">Medea and engineered underedominance </t>
-  </si>
-  <si>
     <t>https://doi.org/10.1111/j.1752-4571.2010.00153.x</t>
   </si>
   <si>
@@ -347,15 +288,9 @@
     <t>" Results show that patchy release generally requires the release of fewer engineered insects to achieve success than central release. "</t>
   </si>
   <si>
-    <t>Emperical data</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
-    <t xml:space="preserve">Y. Huang, K. Magori, A. L. Lloyd, and F. Gould, “Introducing transgenes into insect populations using combined gene-drive strategies: Modeling and analysis,” Insect Biochemistry and Molecular Biology, vol. 37, pp. 1054– 1063, Oct. 2007. </t>
-  </si>
-  <si>
     <t>https://doi.org/10.1016/j.ibmb.2007.06.002</t>
   </si>
   <si>
@@ -401,9 +336,6 @@
     <t>homing endonuclease genes, transposable elements, Medea elements, the intracellular bacterium Wolbachia, engineered underdominance genes, and meiotic drive</t>
   </si>
   <si>
-    <t>"we develop stochastic models to analyze the loss probabilities for several gene drive mechanisms, including homing endonuclease genes, transposable elements, Medea elements, the intracellular bacterium Wolbachia, engineered underdominance genes, and meiotic drive."</t>
-  </si>
-  <si>
     <t xml:space="preserve">J. Min, C. Noble, D. Najjar, and K. Esvelt, “Daisy quorum drives for the genetic restoration of wild populations,” Mar. 2017. </t>
   </si>
   <si>
@@ -434,9 +366,6 @@
     <t xml:space="preserve">C. Noble, J. Olejarz, K. M. Esvelt, G. M. Church, and M. A. Nowak, “Evolutionary dynamics of CRISPR gene drives,” Science Advances, vol. 3, p. e1601964, Apr. 2017. </t>
   </si>
   <si>
-    <t>"we constructed and analyzed a mathematical model of CRISPR gene drive that includes multiplex cutting via multiple gRNAs and allows for multiple costly and cost-free resistant alleles. "</t>
-  </si>
-  <si>
     <t>"we concluded that this architecture could substantially improve the stability of CRISPR gene drives by minimizing the effects of NHEJ-mediated resistance."</t>
   </si>
   <si>
@@ -446,9 +375,6 @@
     <t>https://doi.org/10.1073/pnas.1716358116</t>
   </si>
   <si>
-    <t>"We develop mathematical models which suggest that daisy-chain-drive systems will not spread indefi- nitely through successive populations, and we report numer- ous CRISPR targeting sequences which could offer enhanced stability."</t>
-  </si>
-  <si>
     <t>See Appendix for analysis of equations</t>
   </si>
   <si>
@@ -497,12 +423,6 @@
     <t>https://doi.org/10.1534/genetics.116.197285</t>
   </si>
   <si>
-    <t xml:space="preserve">" we develop a population genetic framework for modeling CGD dynamics, which incorporates potential resistance mechanisms as well as random genetic drift." </t>
-  </si>
-  <si>
-    <t>G. Backus and K. Gross, “Genetic engineering to eradicate invasive mice on islands: Modeling the efficiency and ecological impacts,” Ecosphere, vol. 7, no. 12, 2016.</t>
-  </si>
-  <si>
     <t>https://doi.org/10.1002/ecs2.1589</t>
   </si>
   <si>
@@ -551,9 +471,6 @@
     <t>https://doi.org/10.1073/pnas.1611064114</t>
   </si>
   <si>
-    <t>"mathematical model to analyze the population dynamics of eradication with this genetically engineered mouse and determined its eradication efficiency through model analysis and simulations."</t>
-  </si>
-  <si>
     <t xml:space="preserve">M. Edgington and L. Alphey, “Population dynamics of engineered under- dominance and killer rescue gene drives in the control of disease vectors,” PLoS Computational Biology, vol. 14, no. 3, 2018. </t>
   </si>
   <si>
@@ -675,27 +592,18 @@
   </si>
   <si>
     <t>https://doi.org/10.1101/728006</t>
-  </si>
-  <si>
-    <t>Biorxiv</t>
   </si>
   <si>
     <t>"Here we use simple models to show that spatial structure in the vector population can greatly
 facilitate persistence and evolution of resistance by the disease agent."</t>
   </si>
   <si>
-    <t>ArXiv</t>
-  </si>
-  <si>
     <t>Calvez V, Débarre F, Girardin L. Catch me if you can: a spatial model for a brake-driven gene drive reversal. arXiv preprint arXiv:1812.06641. 2018 Dec 17.</t>
   </si>
   <si>
     <t>"Our results indicate that some drives may be unstoppable, and that, if gene drives are ever deployed in nature, threshold drives, that only spread if introduced in high enough frequencies, should be preferred."</t>
   </si>
   <si>
-    <t>"Here, we consider a reaction-diffusion system modeling the release of a gene drive (of fitness 1 − a) and a brake (fitness 1 − b, b ≤ a) in a wild-type population (fitness 1)."</t>
-  </si>
-  <si>
     <t>Female fertility homing drive, Both-sex fertility drive, Driving Y, Toxin-Antidote Dominant Sperm suppression drive</t>
   </si>
   <si>
@@ -759,9 +667,6 @@
     <t>https://doi.org/10.1126/sciadv.aau8462</t>
   </si>
   <si>
-    <t>"We analyze a statistically representative survey (n = 1018) of U.S. adult attitudes toward agricultural gene drives."</t>
-  </si>
-  <si>
     <t>"Uncertain human health and ecological effects are the public’s most important concerns to resolve."</t>
   </si>
   <si>
@@ -795,18 +700,12 @@
     <t>Current Biology</t>
   </si>
   <si>
-    <t>Insect Biochemisry and Molecular Biology</t>
-  </si>
-  <si>
     <t>Journal of Heredity</t>
   </si>
   <si>
     <t>Journal of Theoretical Biology</t>
   </si>
   <si>
-    <t>BioX</t>
-  </si>
-  <si>
     <t>Peer reviewed</t>
   </si>
   <si>
@@ -972,9 +871,6 @@
     <t>Underdominance</t>
   </si>
   <si>
-    <t>Heffel MG, Finnigan GC. Mathematical modeling of self-contained CRISPR gene drive reversal systems. Scientific Reports. 2019 Dec 27;9(1):1-0.</t>
-  </si>
-  <si>
     <t>https://doi.org/10.1038/s41598-019-54805-8</t>
   </si>
   <si>
@@ -1003,6 +899,107 @@
   </si>
   <si>
     <t>Underdominance - CRISPR, Maternal effect, reciprocal translocation, Haploinsufficient RNA; Wolbachia, CRISPR</t>
+  </si>
+  <si>
+    <t>Aim of the Study (Suppression/replacement)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Empirical data in modelling. Sub Sharan Africa. Namawala (Tanzania) and Garki (Nigeria)  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Studied the effect of realistic seasonality in contrast to non-seasonality on vector population dynamics. Seasonality helps gene drive spread. Explored effect of spatial pattern, release timing, frequency, and migration rate on spread of malaria for 3 gene drive approaches (1) population suppression (2) Driving Y (3) Population replacement. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">how three different gene drive tech- niques—population suppression through dual-germline fertility disruption, population suppression with a driving-Y chromo- some, and population replacement—would fare upon release in two well-studied, field data-rich, and previously modelled settings. </t>
+  </si>
+  <si>
+    <t>Epidemiological modelling takes into account stochasticity, vector populations, larval dynamics, Adult feeding behaviour, closed egg laying, spatial for human and vectors, migration, data from sub-Saharan Africa</t>
+  </si>
+  <si>
+    <t>Aim - Analytical modelling to evaluate the efficiency of synthetic resistance, reversal drives and immunizing reversal drives in eliminating HD. Countermeasures against the spread of drive alleles</t>
+  </si>
+  <si>
+    <t>Synthetic resistance and reversal drives are unlikely to prevent Homing drive fixation because of stable polymorphic equilibrium. Immunizing Reversal Drives (IRD) theoretically ensure elimination of HD. But Cas9 remains</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> Ref 17-19 "Lyttle’s caged popular- tions of </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Drosophila" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Ref 21: " supported by a new flour beetle study analysing pre-existing DNA sequence variation in genomic sites that would be prime candidates for CRISPR-Cas9 GDSs "</t>
+    </r>
+  </si>
+  <si>
+    <t>Experiment to demonstrate the gRNA multiplexing as mechanism against gene drive resistance.</t>
+  </si>
+  <si>
+    <t>"Here, we use a population genetics model to compare the expected characteristics of three spatially self-limiting gene drive systems: one-locus underdominance, two-locus underdominance and daisy chain drives. We find large differences b"</t>
+  </si>
+  <si>
+    <t>New Zealand, gene drive system, risks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medea and engineered underdominance </t>
+  </si>
+  <si>
+    <t>Empirical data</t>
+  </si>
+  <si>
+    <t>Insect Biochemistry and Molecular Biology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y. Huang, K. Magori, A. L. Lloyd, and F. Gould, “Introducing transgenes into insect populations using combined gene-drive strategies: Modelling and analysis,” Insect Biochemistry and Molecular Biology, vol. 37, pp. 1054– 1063, Oct. 2007. </t>
+  </si>
+  <si>
+    <t>"we develop stochastic models to analyse the loss probabilities for several gene drive mechanisms, including homing endonuclease genes, transposable elements, Medea elements, the intracellular bacterium Wolbachia, engineered underdominance genes, and meiotic drive."</t>
+  </si>
+  <si>
+    <t>"we constructed and analysed a mathematical model of CRISPR gene drive that includes multiplex cutting via multiple gRNAs and allows for multiple costly and cost-free resistant alleles. "</t>
+  </si>
+  <si>
+    <t>"We develop mathematical models which suggest that daisy-chain-drive systems will not spread indefi- nitely through successive populations, and we report number- ous CRISPR targeting sequences which could offer enhanced stability."</t>
+  </si>
+  <si>
+    <t xml:space="preserve">" we develop a population genetic framework for modelling CGD dynamics, which incorporates potential resistance mechanisms as well as random genetic drift." </t>
+  </si>
+  <si>
+    <t>G. Backus and K. Gross, “Genetic engineering to eradicate invasive mice on islands: Modelling the efficiency and ecological impacts,” Ecosphere, vol. 7, no. 12, 2016.</t>
+  </si>
+  <si>
+    <t>"mathematical model to analyse the population dynamics of eradication with this genetically engineered mouse and determined its eradication efficiency through model analysis and simulations."</t>
+  </si>
+  <si>
+    <t>"Here, we consider a reaction-diffusion system modelling the release of a gene drive (of fitness 1 − a) and a brake (fitness 1 − b, b ≤ a) in a wild-type population (fitness 1)."</t>
+  </si>
+  <si>
+    <t>"We analyse a statistically representative survey (n = 1018) of U.S. adult attitudes toward agricultural gene drives."</t>
+  </si>
+  <si>
+    <t>Heffel MG, Finnigan GC. Mathematical modelling of self-contained CRISPR gene drive reversal systems. Scientific Reports. 2019 Dec 27;9(1):1-0.</t>
+  </si>
+  <si>
+    <t>arXiv</t>
+  </si>
+  <si>
+    <t>bioRxiv</t>
   </si>
 </sst>
 </file>
@@ -4181,7 +4178,7 @@
   <dimension ref="A1:U66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55:B56"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4231,31 +4228,31 @@
     </row>
     <row r="2" spans="1:21" s="7" customFormat="1" ht="51">
       <c r="A2" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>304</v>
+        <v>277</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>306</v>
+        <v>279</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>305</v>
+        <v>278</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
       <c r="G2" s="15" t="s">
         <v>9</v>
       </c>
       <c r="H2" s="15" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="I2" s="55" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J2" s="6" t="s">
         <v>1</v>
@@ -4276,7 +4273,7 @@
         <v>5</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>10</v>
+        <v>281</v>
       </c>
       <c r="Q2" s="5" t="s">
         <v>7</v>
@@ -4299,13 +4296,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>229</v>
+        <v>205</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="E3" s="33">
         <v>1</v>
@@ -4314,22 +4311,22 @@
         <v>2017</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>184</v>
+        <v>164</v>
       </c>
       <c r="H3" s="29" t="s">
-        <v>156</v>
+        <v>137</v>
       </c>
       <c r="I3" s="54">
         <v>70</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>18</v>
+        <v>282</v>
       </c>
       <c r="M3" s="3">
         <v>0</v>
@@ -4341,22 +4338,22 @@
         <v>1</v>
       </c>
       <c r="P3" s="10" t="s">
-        <v>259</v>
+        <v>233</v>
       </c>
       <c r="Q3" s="10">
         <v>1</v>
       </c>
       <c r="R3" s="8" t="s">
-        <v>22</v>
+        <v>283</v>
       </c>
       <c r="S3" s="17" t="s">
-        <v>13</v>
+        <v>284</v>
       </c>
       <c r="T3" s="9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="U3" s="4" t="s">
-        <v>15</v>
+        <v>285</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="94" customHeight="1">
@@ -4365,10 +4362,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>230</v>
+        <v>206</v>
       </c>
       <c r="D4" s="10">
         <v>1</v>
@@ -4380,22 +4377,22 @@
         <v>2018</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H4" s="21" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I4" s="56">
         <v>100</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="M4" s="3">
         <v>0</v>
@@ -4407,13 +4404,13 @@
         <v>1</v>
       </c>
       <c r="P4" s="38" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="Q4" s="10">
         <v>1</v>
       </c>
       <c r="R4" s="13" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="S4" s="3"/>
       <c r="T4" s="3"/>
@@ -4425,10 +4422,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>231</v>
+        <v>207</v>
       </c>
       <c r="D5" s="10">
         <v>1</v>
@@ -4440,22 +4437,22 @@
         <v>2017</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H5" s="21" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="I5" s="56">
         <v>100</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="M5" s="3">
         <v>1</v>
@@ -4467,16 +4464,16 @@
         <v>0</v>
       </c>
       <c r="P5" s="10" t="s">
-        <v>259</v>
+        <v>233</v>
       </c>
       <c r="Q5" s="10">
         <v>1</v>
       </c>
       <c r="R5" s="13" t="s">
-        <v>24</v>
+        <v>286</v>
       </c>
       <c r="S5" s="19" t="s">
-        <v>25</v>
+        <v>287</v>
       </c>
       <c r="T5" s="1"/>
       <c r="U5" s="1"/>
@@ -4487,13 +4484,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>229</v>
+        <v>205</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="E6" s="34">
         <v>1</v>
@@ -4502,49 +4499,49 @@
         <v>2019</v>
       </c>
       <c r="G6" s="20" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="H6" s="21" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="I6" s="56" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="J6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M6" s="3">
+        <v>0</v>
+      </c>
+      <c r="N6" s="3">
+        <v>0</v>
+      </c>
+      <c r="O6" s="3">
+        <v>0</v>
+      </c>
+      <c r="P6" s="78" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="R6" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="S6" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="T6" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="K6" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="M6" s="3">
-        <v>0</v>
-      </c>
-      <c r="N6" s="3">
-        <v>0</v>
-      </c>
-      <c r="O6" s="3">
-        <v>0</v>
-      </c>
-      <c r="P6" s="78" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="R6" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="S6" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="T6" s="17" t="s">
-        <v>26</v>
-      </c>
       <c r="U6" s="1" t="s">
-        <v>185</v>
+        <v>165</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="126" customHeight="1">
@@ -4553,13 +4550,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>229</v>
+        <v>205</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="E7" s="3">
         <v>1</v>
@@ -4568,22 +4565,22 @@
         <v>2018</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="H7" s="21" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="I7" s="56">
         <v>10</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>257</v>
+        <v>231</v>
       </c>
       <c r="K7" s="11" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="M7" s="3">
         <v>0</v>
@@ -4595,16 +4592,16 @@
         <v>0</v>
       </c>
       <c r="P7" s="38" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="Q7" s="10">
         <v>1</v>
       </c>
       <c r="R7" s="13" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="S7" s="14" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="T7" s="13"/>
       <c r="U7" s="1"/>
@@ -4615,10 +4612,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>232</v>
+        <v>208</v>
       </c>
       <c r="D8" s="3">
         <v>1</v>
@@ -4630,22 +4627,22 @@
         <v>2017</v>
       </c>
       <c r="G8" s="17" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="H8" s="21" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="I8" s="56" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="K8" s="11" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="L8" s="10" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="M8" s="3">
         <v>0</v>
@@ -4657,22 +4654,22 @@
         <v>0</v>
       </c>
       <c r="P8" s="10" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="R8" s="13" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="S8" s="13" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="T8" s="8" t="s">
-        <v>48</v>
+        <v>288</v>
       </c>
       <c r="U8" s="17" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="107" customHeight="1">
@@ -4681,10 +4678,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="C9" s="37" t="s">
-        <v>233</v>
+        <v>209</v>
       </c>
       <c r="D9" s="25">
         <v>0</v>
@@ -4696,22 +4693,22 @@
         <v>2016</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="H9" s="21" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="I9" s="56" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="K9" s="23" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="M9" s="3">
         <v>0</v>
@@ -4723,16 +4720,16 @@
         <v>0</v>
       </c>
       <c r="P9" s="3" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="Q9" s="10">
         <v>1</v>
       </c>
       <c r="R9" s="24" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="S9" s="22" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
@@ -4743,13 +4740,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>229</v>
+        <v>205</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="E10" s="3">
         <v>1</v>
@@ -4758,22 +4755,22 @@
         <v>2018</v>
       </c>
       <c r="G10" s="45" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="H10" s="21" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="I10" s="56">
         <v>10</v>
       </c>
       <c r="J10" s="38" t="s">
-        <v>257</v>
+        <v>231</v>
       </c>
       <c r="K10" s="11" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="M10" s="3">
         <v>0</v>
@@ -4785,16 +4782,16 @@
         <v>0</v>
       </c>
       <c r="P10" s="10" t="s">
-        <v>60</v>
+        <v>289</v>
       </c>
       <c r="Q10" s="3">
         <v>1</v>
       </c>
       <c r="R10" s="26" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="S10" s="27" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="T10" s="13"/>
       <c r="U10" s="13"/>
@@ -4805,10 +4802,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>234</v>
+        <v>210</v>
       </c>
       <c r="D11" s="3">
         <v>1</v>
@@ -4820,22 +4817,22 @@
         <v>2018</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="H11" s="21" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="I11" s="56">
         <v>100</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="K11" s="11" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="M11" s="3">
         <v>1</v>
@@ -4847,19 +4844,19 @@
         <v>1</v>
       </c>
       <c r="P11" s="16" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="Q11" s="10">
         <v>1</v>
       </c>
       <c r="R11" s="13" t="s">
-        <v>65</v>
+        <v>290</v>
       </c>
       <c r="S11" s="13" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="T11" s="13" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="U11" s="13"/>
     </row>
@@ -4869,10 +4866,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>230</v>
+        <v>206</v>
       </c>
       <c r="D12" s="3">
         <v>1</v>
@@ -4884,22 +4881,22 @@
         <v>2014</v>
       </c>
       <c r="G12" s="45" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="H12" s="21" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="I12" s="56" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="J12" s="28" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="K12" s="11" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="M12" s="3">
         <v>0</v>
@@ -4911,13 +4908,13 @@
         <v>0</v>
       </c>
       <c r="P12" s="78" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="Q12" s="3">
         <v>1</v>
       </c>
       <c r="R12" s="13" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="S12" s="13"/>
       <c r="T12" s="13"/>
@@ -4929,10 +4926,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>235</v>
+        <v>211</v>
       </c>
       <c r="D13" s="3">
         <v>1</v>
@@ -4944,22 +4941,22 @@
         <v>2017</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="H13" s="29" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="I13" s="56" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="K13" s="11" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="M13" s="3">
         <v>0</v>
@@ -4971,16 +4968,16 @@
         <v>0</v>
       </c>
       <c r="P13" s="78" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="Q13" s="3">
         <v>1</v>
       </c>
       <c r="R13" s="13" t="s">
-        <v>74</v>
+        <v>291</v>
       </c>
       <c r="S13" s="13" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="T13" s="13"/>
       <c r="U13" s="13"/>
@@ -4991,10 +4988,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>236</v>
+        <v>212</v>
       </c>
       <c r="D14" s="3">
         <v>1</v>
@@ -5006,22 +5003,22 @@
         <v>2017</v>
       </c>
       <c r="G14" s="45" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="H14" s="29" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="I14" s="54">
         <v>90</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="K14" s="11" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="M14" s="3">
         <v>1</v>
@@ -5033,13 +5030,13 @@
         <v>1</v>
       </c>
       <c r="P14" s="3" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="Q14" s="3">
         <v>1</v>
       </c>
       <c r="R14" s="13" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="S14" s="13"/>
       <c r="T14" s="13"/>
@@ -5051,13 +5048,13 @@
         <v>13</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>237</v>
+        <v>213</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="E15" s="10">
         <v>1</v>
@@ -5066,22 +5063,22 @@
         <v>2013</v>
       </c>
       <c r="G15" s="45" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="H15" s="29" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="I15" s="56">
         <v>30</v>
       </c>
       <c r="J15" s="38" t="s">
-        <v>257</v>
+        <v>231</v>
       </c>
       <c r="K15" s="12" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="M15" s="3">
         <v>1</v>
@@ -5093,19 +5090,19 @@
         <v>1</v>
       </c>
       <c r="P15" s="10" t="s">
-        <v>259</v>
+        <v>233</v>
       </c>
       <c r="Q15" s="3">
         <v>1</v>
       </c>
       <c r="R15" s="13" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="S15" s="13" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="T15" s="13" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="U15" s="13"/>
     </row>
@@ -5115,10 +5112,10 @@
         <v>14</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>234</v>
+        <v>210</v>
       </c>
       <c r="D16" s="3">
         <v>1</v>
@@ -5130,22 +5127,22 @@
         <v>2011</v>
       </c>
       <c r="G16" s="45" t="s">
-        <v>183</v>
+        <v>163</v>
       </c>
       <c r="H16" s="29" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="I16" s="56">
         <v>80</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="K16" s="12" t="s">
-        <v>85</v>
+        <v>292</v>
       </c>
       <c r="L16" s="10" t="s">
-        <v>89</v>
+        <v>293</v>
       </c>
       <c r="M16" s="3">
         <v>1</v>
@@ -5157,16 +5154,16 @@
         <v>1</v>
       </c>
       <c r="P16" s="3" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="Q16" s="3">
         <v>0</v>
       </c>
       <c r="R16" s="13" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="S16" s="13" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="T16" s="13"/>
       <c r="U16" s="13"/>
@@ -5177,10 +5174,10 @@
         <v>15</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>238</v>
+        <v>294</v>
       </c>
       <c r="D17" s="3">
         <v>0</v>
@@ -5192,22 +5189,22 @@
         <v>2007</v>
       </c>
       <c r="G17" s="31" t="s">
-        <v>91</v>
+        <v>295</v>
       </c>
       <c r="H17" s="29" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="I17" s="56">
         <v>80</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="K17" s="30" t="s">
-        <v>167</v>
+        <v>147</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="M17" s="3">
         <v>1</v>
@@ -5219,16 +5216,16 @@
         <v>0</v>
       </c>
       <c r="P17" s="3" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="Q17" s="3">
         <v>0</v>
       </c>
       <c r="R17" s="13" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="S17" s="13" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="T17" s="13"/>
       <c r="U17" s="13"/>
@@ -5239,10 +5236,10 @@
         <v>16</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>231</v>
+        <v>207</v>
       </c>
       <c r="D18" s="10">
         <v>1</v>
@@ -5254,22 +5251,22 @@
         <v>2017</v>
       </c>
       <c r="G18" s="19" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="H18" s="29" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="I18" s="56">
         <v>70</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="K18" s="11" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="M18" s="3">
         <v>1</v>
@@ -5281,16 +5278,16 @@
         <v>0</v>
       </c>
       <c r="P18" s="38" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="Q18" s="10">
         <v>1</v>
       </c>
       <c r="R18" s="13" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="S18" s="13" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="T18" s="13"/>
       <c r="U18" s="13"/>
@@ -5301,13 +5298,13 @@
         <v>17</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>239</v>
+        <v>214</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="E19" s="3">
         <v>1</v>
@@ -5316,22 +5313,22 @@
         <v>2011</v>
       </c>
       <c r="G19" s="17" t="s">
-        <v>181</v>
+        <v>161</v>
       </c>
       <c r="H19" s="29" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="I19" s="56">
         <v>70</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="K19" s="11" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="M19" s="3">
         <v>1</v>
@@ -5343,16 +5340,16 @@
         <v>1</v>
       </c>
       <c r="P19" s="3" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="Q19" s="3">
         <v>0</v>
       </c>
       <c r="R19" s="13" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="S19" s="13" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="T19" s="13"/>
       <c r="U19" s="13"/>
@@ -5363,10 +5360,10 @@
         <v>18</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>240</v>
+        <v>215</v>
       </c>
       <c r="D20" s="3">
         <v>0</v>
@@ -5378,22 +5375,22 @@
         <v>2009</v>
       </c>
       <c r="G20" s="20" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="H20" s="29" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="I20" s="56">
         <v>90</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="K20" s="32" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="M20" s="3">
         <v>0</v>
@@ -5405,13 +5402,13 @@
         <v>0</v>
       </c>
       <c r="P20" s="10" t="s">
-        <v>259</v>
+        <v>233</v>
       </c>
       <c r="Q20" s="3">
         <v>0</v>
       </c>
       <c r="R20" s="13" t="s">
-        <v>107</v>
+        <v>296</v>
       </c>
       <c r="S20" s="13"/>
       <c r="T20" s="13"/>
@@ -5423,10 +5420,10 @@
         <v>19</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>244</v>
+        <v>218</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>241</v>
+        <v>306</v>
       </c>
       <c r="D21" s="3">
         <v>1</v>
@@ -5438,22 +5435,22 @@
         <v>2017</v>
       </c>
       <c r="G21" s="17" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="H21" s="21" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="I21" s="56">
         <v>40</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="K21" s="11" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="M21" s="3">
         <v>0</v>
@@ -5465,16 +5462,16 @@
         <v>0</v>
       </c>
       <c r="P21" s="10" t="s">
-        <v>259</v>
+        <v>233</v>
       </c>
       <c r="Q21" s="3">
         <v>0</v>
       </c>
       <c r="R21" s="8" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="S21" s="13" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="T21" s="13"/>
       <c r="U21" s="13"/>
@@ -5485,10 +5482,10 @@
         <v>20</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>243</v>
+        <v>217</v>
       </c>
       <c r="D22" s="3">
         <v>1</v>
@@ -5500,22 +5497,22 @@
         <v>2019</v>
       </c>
       <c r="G22" s="17" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="H22" s="40" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="I22" s="56">
         <v>70</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="K22" s="11" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="L22" s="10" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="M22" s="3">
         <v>1</v>
@@ -5527,13 +5524,13 @@
         <v>0</v>
       </c>
       <c r="P22" s="3" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="Q22" s="10">
         <v>1</v>
       </c>
       <c r="R22" s="13" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="S22" s="13"/>
       <c r="T22" s="13"/>
@@ -5545,10 +5542,10 @@
         <v>21</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>245</v>
+        <v>219</v>
       </c>
       <c r="D23" s="3">
         <v>1</v>
@@ -5560,22 +5557,22 @@
         <v>2017</v>
       </c>
       <c r="G23" s="17" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="H23" s="18" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="I23" s="56">
         <v>90</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="K23" s="11" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="M23" s="3">
         <v>1</v>
@@ -5587,16 +5584,16 @@
         <v>0</v>
       </c>
       <c r="P23" s="3" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="Q23" s="3">
         <v>1</v>
       </c>
       <c r="R23" s="13" t="s">
-        <v>118</v>
+        <v>297</v>
       </c>
       <c r="S23" s="13" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="T23" s="13"/>
       <c r="U23" s="13"/>
@@ -5607,13 +5604,13 @@
         <v>22</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>229</v>
+        <v>205</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="E24" s="3">
         <v>1</v>
@@ -5622,22 +5619,22 @@
         <v>2019</v>
       </c>
       <c r="G24" s="17" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="H24" s="29" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="I24" s="56">
         <v>80</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="K24" s="11" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="M24" s="3">
         <v>1</v>
@@ -5649,16 +5646,16 @@
         <v>1</v>
       </c>
       <c r="P24" s="3" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="Q24" s="3">
         <v>1</v>
       </c>
       <c r="R24" s="13" t="s">
-        <v>122</v>
+        <v>298</v>
       </c>
       <c r="S24" s="13" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
       <c r="T24" s="13"/>
       <c r="U24" s="13"/>
@@ -5669,13 +5666,13 @@
         <v>23</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>229</v>
+        <v>205</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="E25" s="3">
         <v>1</v>
@@ -5684,22 +5681,22 @@
         <v>2018</v>
       </c>
       <c r="G25" s="17" t="s">
-        <v>124</v>
+        <v>107</v>
       </c>
       <c r="H25" s="29" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="I25" s="56">
         <v>30</v>
       </c>
       <c r="J25" s="38" t="s">
-        <v>257</v>
+        <v>231</v>
       </c>
       <c r="K25" s="11" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="L25" s="3" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="M25" s="3">
         <v>1</v>
@@ -5711,19 +5708,19 @@
         <v>0</v>
       </c>
       <c r="P25" s="3" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="Q25" s="3">
         <v>1</v>
       </c>
       <c r="R25" s="13" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
       <c r="S25" s="13" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
       <c r="T25" s="13" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="U25" s="13"/>
     </row>
@@ -5733,13 +5730,13 @@
         <v>24</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>229</v>
+        <v>205</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="E26" s="3">
         <v>1</v>
@@ -5748,22 +5745,22 @@
         <v>2019</v>
       </c>
       <c r="G26" s="17" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="H26" s="29" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="I26" s="56">
         <v>30</v>
       </c>
       <c r="J26" s="38" t="s">
-        <v>257</v>
+        <v>231</v>
       </c>
       <c r="K26" s="11" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="L26" s="3" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="M26" s="3">
         <v>1</v>
@@ -5775,13 +5772,13 @@
         <v>0</v>
       </c>
       <c r="P26" s="3" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="Q26" s="3">
         <v>1</v>
       </c>
       <c r="R26" s="13" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="S26" s="13"/>
       <c r="T26" s="13"/>
@@ -5793,13 +5790,13 @@
         <v>25</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>229</v>
+        <v>205</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="E27" s="3">
         <v>1</v>
@@ -5808,22 +5805,22 @@
         <v>2017</v>
       </c>
       <c r="G27" s="17" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
       <c r="H27" s="29" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="I27" s="56">
         <v>90</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="K27" s="11" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="M27" s="3">
         <v>1</v>
@@ -5835,16 +5832,16 @@
         <v>1</v>
       </c>
       <c r="P27" s="3" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="Q27" s="3">
         <v>0</v>
       </c>
       <c r="R27" s="13" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="S27" s="13" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
       <c r="T27" s="13"/>
       <c r="U27" s="13"/>
@@ -5855,13 +5852,13 @@
         <v>26</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>246</v>
+        <v>220</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="E28" s="3">
         <v>0</v>
@@ -5870,22 +5867,22 @@
         <v>2017</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="H28" s="29" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
       <c r="I28" s="56">
         <v>90</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="K28" s="11" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="L28" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="M28" s="3">
         <v>1</v>
@@ -5897,13 +5894,13 @@
         <v>0</v>
       </c>
       <c r="P28" s="3" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="Q28" s="3">
         <v>1</v>
       </c>
       <c r="R28" s="13" t="s">
-        <v>139</v>
+        <v>299</v>
       </c>
       <c r="S28" s="13"/>
       <c r="T28" s="13"/>
@@ -5915,10 +5912,10 @@
         <v>27</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>247</v>
+        <v>221</v>
       </c>
       <c r="D29" s="3">
         <v>1</v>
@@ -5930,22 +5927,22 @@
         <v>2016</v>
       </c>
       <c r="G29" s="35" t="s">
-        <v>140</v>
+        <v>300</v>
       </c>
       <c r="H29" s="21" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
       <c r="I29" s="56">
         <v>90</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="K29" s="58" t="s">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="L29" s="10" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="M29" s="3">
         <v>1</v>
@@ -5957,13 +5954,13 @@
         <v>0</v>
       </c>
       <c r="P29" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="Q29" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="R29" s="13" t="s">
-        <v>157</v>
+        <v>301</v>
       </c>
       <c r="S29" s="13"/>
       <c r="T29" s="13"/>
@@ -5975,10 +5972,10 @@
         <v>28</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>248</v>
+        <v>222</v>
       </c>
       <c r="D30" s="3">
         <v>1</v>
@@ -5990,22 +5987,22 @@
         <v>2018</v>
       </c>
       <c r="G30" s="17" t="s">
-        <v>158</v>
+        <v>138</v>
       </c>
       <c r="H30" s="29" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
       <c r="I30" s="56">
         <v>90</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="K30" s="41" t="s">
-        <v>159</v>
+        <v>139</v>
       </c>
       <c r="L30" s="10" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="M30" s="3">
         <v>1</v>
@@ -6017,19 +6014,19 @@
         <v>1</v>
       </c>
       <c r="P30" s="10" t="s">
-        <v>259</v>
+        <v>233</v>
       </c>
       <c r="Q30" s="3">
         <v>0</v>
       </c>
       <c r="R30" s="13" t="s">
-        <v>161</v>
+        <v>141</v>
       </c>
       <c r="S30" s="13" t="s">
-        <v>162</v>
+        <v>142</v>
       </c>
       <c r="T30" s="13" t="s">
-        <v>163</v>
+        <v>143</v>
       </c>
       <c r="U30" s="13"/>
     </row>
@@ -6039,10 +6036,10 @@
         <v>29</v>
       </c>
       <c r="B31" s="37" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="C31" s="37" t="s">
-        <v>249</v>
+        <v>223</v>
       </c>
       <c r="D31" s="25">
         <v>0</v>
@@ -6054,22 +6051,22 @@
         <v>2018</v>
       </c>
       <c r="G31" s="19" t="s">
-        <v>143</v>
+        <v>124</v>
       </c>
       <c r="H31" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="I31" s="56" t="s">
+        <v>44</v>
+      </c>
+      <c r="J31" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="K31" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="I31" s="56" t="s">
-        <v>52</v>
-      </c>
-      <c r="J31" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="K31" s="12" t="s">
-        <v>164</v>
-      </c>
       <c r="L31" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="M31" s="3">
         <v>0</v>
@@ -6081,16 +6078,16 @@
         <v>0</v>
       </c>
       <c r="P31" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="Q31" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="R31" s="13" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
       <c r="S31" s="13" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
       <c r="T31" s="13"/>
       <c r="U31" s="13"/>
@@ -6101,13 +6098,13 @@
         <v>30</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>229</v>
+        <v>205</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="E32" s="3">
         <v>1</v>
@@ -6116,22 +6113,22 @@
         <v>2018</v>
       </c>
       <c r="G32" s="36" t="s">
-        <v>182</v>
+        <v>162</v>
       </c>
       <c r="H32" s="29" t="s">
-        <v>145</v>
+        <v>126</v>
       </c>
       <c r="I32" s="56">
         <v>60</v>
       </c>
       <c r="J32" s="38" t="s">
-        <v>257</v>
+        <v>231</v>
       </c>
       <c r="K32" s="11" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="L32" s="10" t="s">
-        <v>169</v>
+        <v>149</v>
       </c>
       <c r="M32" s="3">
         <v>1</v>
@@ -6143,13 +6140,13 @@
         <v>0</v>
       </c>
       <c r="P32" s="38" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="Q32" s="3">
         <v>1</v>
       </c>
       <c r="R32" s="13" t="s">
-        <v>168</v>
+        <v>148</v>
       </c>
       <c r="S32" s="13"/>
       <c r="T32" s="13"/>
@@ -6161,13 +6158,13 @@
         <v>31</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>250</v>
+        <v>224</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="E33" s="3">
         <v>1</v>
@@ -6176,22 +6173,22 @@
         <v>2018</v>
       </c>
       <c r="G33" s="17" t="s">
-        <v>147</v>
+        <v>128</v>
       </c>
       <c r="H33" s="38" t="s">
-        <v>146</v>
+        <v>127</v>
       </c>
       <c r="I33" s="54">
         <v>80</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="K33" s="12" t="s">
-        <v>307</v>
+        <v>280</v>
       </c>
       <c r="L33" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="M33" s="3">
         <v>0</v>
@@ -6203,19 +6200,19 @@
         <v>0</v>
       </c>
       <c r="P33" s="10" t="s">
-        <v>259</v>
+        <v>233</v>
       </c>
       <c r="Q33" s="3">
         <v>0</v>
       </c>
       <c r="R33" s="13" t="s">
-        <v>170</v>
+        <v>150</v>
       </c>
       <c r="S33" s="13" t="s">
-        <v>171</v>
+        <v>151</v>
       </c>
       <c r="T33" s="13" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
       <c r="U33" s="13"/>
     </row>
@@ -6225,10 +6222,10 @@
         <v>32</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>238</v>
+        <v>294</v>
       </c>
       <c r="D34" s="3">
         <v>0</v>
@@ -6240,22 +6237,22 @@
         <v>2005</v>
       </c>
       <c r="G34" s="17" t="s">
-        <v>148</v>
+        <v>129</v>
       </c>
       <c r="H34" s="29" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
       <c r="I34" s="56">
         <v>90</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="K34" s="43" t="s">
-        <v>174</v>
+        <v>154</v>
       </c>
       <c r="L34" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="M34" s="3">
         <v>0</v>
@@ -6267,13 +6264,13 @@
         <v>0</v>
       </c>
       <c r="P34" s="38" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="Q34" s="3">
         <v>0</v>
       </c>
       <c r="R34" s="42" t="s">
-        <v>173</v>
+        <v>153</v>
       </c>
       <c r="S34" s="13"/>
       <c r="T34" s="13"/>
@@ -6285,10 +6282,10 @@
         <v>33</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>251</v>
+        <v>225</v>
       </c>
       <c r="D35" s="3">
         <v>0</v>
@@ -6300,22 +6297,22 @@
         <v>2005</v>
       </c>
       <c r="G35" s="17" t="s">
-        <v>151</v>
+        <v>132</v>
       </c>
       <c r="H35" s="39" t="s">
-        <v>150</v>
+        <v>131</v>
       </c>
       <c r="I35" s="56">
         <v>100</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="K35" s="44" t="s">
-        <v>174</v>
+        <v>154</v>
       </c>
       <c r="L35" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="M35" s="3">
         <v>1</v>
@@ -6327,13 +6324,13 @@
         <v>0</v>
       </c>
       <c r="P35" s="3" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="Q35" s="3">
         <v>0</v>
       </c>
       <c r="R35" s="13" t="s">
-        <v>175</v>
+        <v>155</v>
       </c>
       <c r="S35" s="13"/>
       <c r="T35" s="13"/>
@@ -6345,10 +6342,10 @@
         <v>34</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>252</v>
+        <v>226</v>
       </c>
       <c r="D36" s="3">
         <v>1</v>
@@ -6360,22 +6357,22 @@
         <v>2018</v>
       </c>
       <c r="G36" s="17" t="s">
-        <v>155</v>
+        <v>136</v>
       </c>
       <c r="H36" s="29" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
       <c r="I36" s="56">
         <v>90</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="K36" s="3" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="L36" s="10" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="M36" s="3">
         <v>1</v>
@@ -6387,16 +6384,16 @@
         <v>1</v>
       </c>
       <c r="P36" s="3" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="Q36" s="3">
         <v>0</v>
       </c>
       <c r="R36" s="13" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
       <c r="S36" s="13" t="s">
-        <v>177</v>
+        <v>157</v>
       </c>
       <c r="T36" s="13"/>
       <c r="U36" s="13"/>
@@ -6407,10 +6404,10 @@
         <v>35</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>253</v>
+        <v>227</v>
       </c>
       <c r="D37" s="3">
         <v>0</v>
@@ -6422,22 +6419,22 @@
         <v>2011</v>
       </c>
       <c r="G37" s="17" t="s">
-        <v>154</v>
+        <v>135</v>
       </c>
       <c r="H37" s="29" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="I37" s="56">
         <v>70</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="K37" s="43" t="s">
-        <v>178</v>
+        <v>158</v>
       </c>
       <c r="L37" s="3" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="M37" s="3">
         <v>1</v>
@@ -6449,13 +6446,13 @@
         <v>0</v>
       </c>
       <c r="P37" s="3" t="s">
-        <v>259</v>
+        <v>233</v>
       </c>
       <c r="Q37" s="3">
         <v>1</v>
       </c>
       <c r="R37" s="13" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
       <c r="S37" s="13"/>
       <c r="T37" s="13"/>
@@ -6467,10 +6464,10 @@
         <v>36</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>245</v>
+        <v>219</v>
       </c>
       <c r="D38" s="3">
         <v>1</v>
@@ -6482,43 +6479,43 @@
         <v>2017</v>
       </c>
       <c r="G38" s="50" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="H38" s="48" t="s">
-        <v>190</v>
+        <v>170</v>
       </c>
       <c r="I38" s="54">
         <v>50</v>
       </c>
       <c r="J38" s="7" t="s">
-        <v>258</v>
+        <v>232</v>
       </c>
       <c r="K38" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="L38" s="10" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
       <c r="M38" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="N38" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="O38" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="P38" s="3" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="Q38" s="10">
         <v>1</v>
       </c>
       <c r="R38" s="46" t="s">
-        <v>192</v>
+        <v>172</v>
       </c>
       <c r="S38" s="13" t="s">
-        <v>193</v>
+        <v>173</v>
       </c>
       <c r="T38" s="13"/>
       <c r="U38" s="13"/>
@@ -6529,10 +6526,10 @@
         <v>37</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>254</v>
+        <v>228</v>
       </c>
       <c r="D39" s="10">
         <v>1</v>
@@ -6544,22 +6541,22 @@
         <v>2017</v>
       </c>
       <c r="G39" s="49" t="s">
-        <v>194</v>
+        <v>174</v>
       </c>
       <c r="H39" s="29" t="s">
-        <v>195</v>
+        <v>175</v>
       </c>
       <c r="I39" s="56">
         <v>100</v>
       </c>
       <c r="J39" s="3" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="K39" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="L39" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="M39" s="3">
         <v>1</v>
@@ -6571,13 +6568,13 @@
         <v>0</v>
       </c>
       <c r="P39" s="3" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="Q39" s="3">
         <v>1</v>
       </c>
       <c r="R39" s="13" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
       <c r="S39" s="13"/>
       <c r="T39" s="13"/>
@@ -6589,10 +6586,10 @@
         <v>38</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>244</v>
+        <v>218</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>199</v>
+        <v>306</v>
       </c>
       <c r="D40" s="3">
         <v>1</v>
@@ -6604,22 +6601,22 @@
         <v>2019</v>
       </c>
       <c r="G40" s="50" t="s">
-        <v>197</v>
+        <v>177</v>
       </c>
       <c r="H40" s="47" t="s">
-        <v>198</v>
+        <v>178</v>
       </c>
       <c r="I40" s="56">
         <v>100</v>
       </c>
       <c r="J40" s="10" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="K40" s="3" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="L40" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="M40" s="3">
         <v>1</v>
@@ -6631,13 +6628,13 @@
         <v>1</v>
       </c>
       <c r="P40" s="3" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="Q40" s="3">
         <v>1</v>
       </c>
       <c r="R40" s="13" t="s">
-        <v>200</v>
+        <v>179</v>
       </c>
       <c r="S40" s="13"/>
       <c r="T40" s="13"/>
@@ -6649,10 +6646,10 @@
         <v>39</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>244</v>
+        <v>218</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>201</v>
+        <v>305</v>
       </c>
       <c r="D41" s="3">
         <v>1</v>
@@ -6664,22 +6661,22 @@
         <v>2018</v>
       </c>
       <c r="G41" s="50" t="s">
-        <v>202</v>
+        <v>180</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="I41" s="56">
         <v>100</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="K41" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="L41" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="M41" s="3">
         <v>1</v>
@@ -6691,16 +6688,16 @@
         <v>1</v>
       </c>
       <c r="P41" s="3" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="Q41" s="3">
         <v>0</v>
       </c>
       <c r="R41" s="13" t="s">
-        <v>204</v>
+        <v>302</v>
       </c>
       <c r="S41" s="13" t="s">
-        <v>203</v>
+        <v>181</v>
       </c>
       <c r="T41" s="13"/>
       <c r="U41" s="13"/>
@@ -6711,10 +6708,10 @@
         <v>40</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>244</v>
+        <v>218</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>199</v>
+        <v>306</v>
       </c>
       <c r="D42" s="3">
         <v>1</v>
@@ -6726,22 +6723,22 @@
         <v>2019</v>
       </c>
       <c r="G42" s="50" t="s">
-        <v>206</v>
+        <v>183</v>
       </c>
       <c r="H42" s="21" t="s">
-        <v>207</v>
+        <v>184</v>
       </c>
       <c r="I42" s="56">
         <v>100</v>
       </c>
       <c r="J42" s="10" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="K42" s="10" t="s">
-        <v>205</v>
+        <v>182</v>
       </c>
       <c r="L42" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="M42" s="3">
         <v>0</v>
@@ -6753,16 +6750,16 @@
         <v>1</v>
       </c>
       <c r="P42" s="3" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="Q42" s="3">
         <v>1</v>
       </c>
       <c r="R42" s="13" t="s">
-        <v>208</v>
+        <v>185</v>
       </c>
       <c r="S42" s="13" t="s">
-        <v>209</v>
+        <v>186</v>
       </c>
       <c r="T42" s="13"/>
       <c r="U42" s="13"/>
@@ -6773,13 +6770,13 @@
         <v>41</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>255</v>
+        <v>229</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="E43" s="3">
         <v>1</v>
@@ -6788,22 +6785,22 @@
         <v>2014</v>
       </c>
       <c r="G43" s="52" t="s">
-        <v>210</v>
+        <v>187</v>
       </c>
       <c r="H43" s="29" t="s">
-        <v>211</v>
+        <v>188</v>
       </c>
       <c r="I43" s="56">
         <v>80</v>
       </c>
       <c r="J43" s="5" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="K43" s="10" t="s">
-        <v>212</v>
+        <v>189</v>
       </c>
       <c r="L43" s="10" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="M43" s="3">
         <v>1</v>
@@ -6815,22 +6812,22 @@
         <v>0</v>
       </c>
       <c r="P43" s="3" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="Q43" s="3">
         <v>0</v>
       </c>
       <c r="R43" s="51" t="s">
-        <v>213</v>
+        <v>190</v>
       </c>
       <c r="S43" s="13" t="s">
-        <v>214</v>
+        <v>191</v>
       </c>
       <c r="T43" s="13" t="s">
-        <v>215</v>
+        <v>192</v>
       </c>
       <c r="U43" s="13" t="s">
-        <v>216</v>
+        <v>193</v>
       </c>
     </row>
     <row r="44" spans="1:21" ht="87" customHeight="1">
@@ -6839,10 +6836,10 @@
         <v>42</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>245</v>
+        <v>219</v>
       </c>
       <c r="D44" s="3">
         <v>1</v>
@@ -6854,22 +6851,22 @@
         <v>2015</v>
       </c>
       <c r="G44" s="49" t="s">
-        <v>217</v>
+        <v>194</v>
       </c>
       <c r="H44" s="53" t="s">
-        <v>218</v>
+        <v>195</v>
       </c>
       <c r="I44" s="56">
         <v>5</v>
       </c>
       <c r="J44" s="38" t="s">
-        <v>257</v>
+        <v>231</v>
       </c>
       <c r="K44" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="L44" s="3" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="M44" s="3">
         <v>0</v>
@@ -6881,13 +6878,13 @@
         <v>0</v>
       </c>
       <c r="P44" s="3" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="Q44" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="R44" s="13" t="s">
-        <v>219</v>
+        <v>196</v>
       </c>
       <c r="S44" s="13"/>
       <c r="T44" s="13"/>
@@ -6899,10 +6896,10 @@
         <v>43</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>256</v>
+        <v>230</v>
       </c>
       <c r="D45" s="3">
         <v>1</v>
@@ -6914,43 +6911,43 @@
         <v>2018</v>
       </c>
       <c r="G45" s="17" t="s">
-        <v>220</v>
+        <v>197</v>
       </c>
       <c r="H45" s="29" t="s">
-        <v>221</v>
+        <v>198</v>
       </c>
       <c r="I45" s="56" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="J45" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="K45" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="L45" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="M45" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="N45" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="O45" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="P45" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="Q45" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="R45" s="13" t="s">
-        <v>222</v>
+        <v>199</v>
       </c>
       <c r="S45" s="13" t="s">
-        <v>223</v>
+        <v>200</v>
       </c>
       <c r="T45" s="13"/>
       <c r="U45" s="13"/>
@@ -6961,10 +6958,10 @@
         <v>44</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>245</v>
+        <v>219</v>
       </c>
       <c r="D46" s="18">
         <v>1</v>
@@ -6976,46 +6973,46 @@
         <v>2019</v>
       </c>
       <c r="G46" s="69" t="s">
-        <v>224</v>
+        <v>201</v>
       </c>
       <c r="H46" s="29" t="s">
-        <v>225</v>
+        <v>202</v>
       </c>
       <c r="I46" s="56">
         <v>5</v>
       </c>
       <c r="J46" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="K46" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="L46" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="M46" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="N46" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="O46" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="P46" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="Q46" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="R46" s="13" t="s">
-        <v>226</v>
+        <v>303</v>
       </c>
       <c r="S46" s="13" t="s">
-        <v>227</v>
+        <v>203</v>
       </c>
       <c r="T46" s="27" t="s">
-        <v>228</v>
+        <v>204</v>
       </c>
       <c r="U46" s="13"/>
     </row>
@@ -7025,10 +7022,10 @@
         <v>45</v>
       </c>
       <c r="B47" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="C47" s="68" t="s">
         <v>242</v>
-      </c>
-      <c r="C47" s="68" t="s">
-        <v>268</v>
       </c>
       <c r="D47" s="18">
         <v>0</v>
@@ -7040,40 +7037,40 @@
         <v>1995</v>
       </c>
       <c r="G47" s="73" t="s">
-        <v>269</v>
+        <v>243</v>
       </c>
       <c r="H47" s="70" t="s">
-        <v>270</v>
+        <v>244</v>
       </c>
       <c r="I47" s="56">
         <v>5</v>
       </c>
       <c r="J47" s="38" t="s">
-        <v>257</v>
+        <v>231</v>
       </c>
       <c r="K47" s="3" t="s">
-        <v>272</v>
+        <v>246</v>
       </c>
       <c r="L47" s="3" t="s">
-        <v>271</v>
+        <v>245</v>
       </c>
       <c r="M47" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="N47" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="O47" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="P47" s="3" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="Q47" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="R47" s="13" t="s">
-        <v>273</v>
+        <v>247</v>
       </c>
       <c r="S47" s="13"/>
       <c r="T47" s="13"/>
@@ -7085,13 +7082,13 @@
         <v>46</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="C48" s="10" t="s">
-        <v>276</v>
+        <v>250</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="E48" s="3">
         <v>1</v>
@@ -7100,19 +7097,19 @@
         <v>2019</v>
       </c>
       <c r="G48" s="74" t="s">
-        <v>274</v>
+        <v>248</v>
       </c>
       <c r="H48" s="29" t="s">
-        <v>275</v>
+        <v>249</v>
       </c>
       <c r="I48" s="56">
         <v>90</v>
       </c>
       <c r="J48" s="3" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="K48" s="75" t="s">
-        <v>302</v>
+        <v>275</v>
       </c>
       <c r="L48" s="3"/>
       <c r="M48" s="3">
@@ -7125,7 +7122,7 @@
         <v>1</v>
       </c>
       <c r="P48" s="3" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="Q48" s="3">
         <v>1</v>
@@ -7141,13 +7138,13 @@
         <v>47</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="C49" s="10" t="s">
-        <v>278</v>
+        <v>252</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="E49" s="3">
         <v>1</v>
@@ -7156,34 +7153,34 @@
         <v>2019</v>
       </c>
       <c r="G49" s="76" t="s">
-        <v>277</v>
+        <v>251</v>
       </c>
       <c r="H49" s="29" t="s">
-        <v>279</v>
+        <v>253</v>
       </c>
       <c r="I49" s="56" t="s">
-        <v>280</v>
+        <v>254</v>
       </c>
       <c r="J49" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="K49" s="3" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="L49" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="M49" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="N49" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="O49" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="P49" s="3" t="s">
-        <v>259</v>
+        <v>233</v>
       </c>
       <c r="Q49" s="3">
         <v>1</v>
@@ -7199,10 +7196,10 @@
         <v>48</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>282</v>
+        <v>256</v>
       </c>
       <c r="D50" s="3">
         <v>1</v>
@@ -7214,22 +7211,22 @@
         <v>2019</v>
       </c>
       <c r="G50" s="17" t="s">
-        <v>283</v>
+        <v>257</v>
       </c>
       <c r="H50" s="47" t="s">
-        <v>281</v>
+        <v>255</v>
       </c>
       <c r="I50" s="56">
         <v>80</v>
       </c>
       <c r="J50" s="3" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="K50" s="3" t="s">
-        <v>284</v>
+        <v>258</v>
       </c>
       <c r="L50" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="M50" s="3">
         <v>1</v>
@@ -7241,7 +7238,7 @@
         <v>1</v>
       </c>
       <c r="P50" s="3" t="s">
-        <v>259</v>
+        <v>233</v>
       </c>
       <c r="Q50" s="3">
         <v>0</v>
@@ -7257,10 +7254,10 @@
         <v>49</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>245</v>
+        <v>219</v>
       </c>
       <c r="D51" s="3">
         <v>1</v>
@@ -7272,34 +7269,34 @@
         <v>2007</v>
       </c>
       <c r="G51" s="17" t="s">
-        <v>285</v>
+        <v>259</v>
       </c>
       <c r="H51" s="29" t="s">
-        <v>286</v>
+        <v>260</v>
       </c>
       <c r="I51" s="56">
         <v>20</v>
       </c>
       <c r="J51" s="3" t="s">
-        <v>257</v>
+        <v>231</v>
       </c>
       <c r="K51" s="10" t="s">
-        <v>287</v>
+        <v>261</v>
       </c>
       <c r="L51" s="3" t="s">
-        <v>271</v>
+        <v>245</v>
       </c>
       <c r="M51" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="N51" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="O51" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="P51" s="3" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="Q51" s="3">
         <v>1</v>
@@ -7315,13 +7312,13 @@
         <v>50</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>289</v>
+        <v>263</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="E52" s="3">
         <v>1</v>
@@ -7330,22 +7327,22 @@
         <v>2020</v>
       </c>
       <c r="G52" s="17" t="s">
-        <v>288</v>
+        <v>262</v>
       </c>
       <c r="H52" s="29" t="s">
-        <v>290</v>
+        <v>264</v>
       </c>
       <c r="I52" s="56">
         <v>80</v>
       </c>
       <c r="J52" s="3" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="K52" s="10" t="s">
-        <v>291</v>
+        <v>265</v>
       </c>
       <c r="L52" s="3" t="s">
-        <v>292</v>
+        <v>266</v>
       </c>
       <c r="M52" s="3">
         <v>1</v>
@@ -7357,7 +7354,7 @@
         <v>1</v>
       </c>
       <c r="P52" s="3" t="s">
-        <v>259</v>
+        <v>233</v>
       </c>
       <c r="Q52" s="3">
         <v>1</v>
@@ -7373,10 +7370,10 @@
         <v>51</v>
       </c>
       <c r="B53" s="11" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="C53" s="10" t="s">
-        <v>295</v>
+        <v>269</v>
       </c>
       <c r="D53" s="3">
         <v>1</v>
@@ -7388,22 +7385,22 @@
         <v>2020</v>
       </c>
       <c r="G53" s="17" t="s">
-        <v>294</v>
+        <v>268</v>
       </c>
       <c r="H53" s="70" t="s">
-        <v>293</v>
+        <v>267</v>
       </c>
       <c r="I53" s="56">
         <v>80</v>
       </c>
       <c r="J53" s="3" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="K53" s="3" t="s">
-        <v>296</v>
+        <v>270</v>
       </c>
       <c r="L53" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="M53" s="3">
         <v>0</v>
@@ -7415,7 +7412,7 @@
         <v>1</v>
       </c>
       <c r="P53" s="3" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="Q53" s="3">
         <v>0</v>
@@ -7431,10 +7428,10 @@
         <v>52</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>231</v>
+        <v>207</v>
       </c>
       <c r="D54" s="3">
         <v>1</v>
@@ -7446,22 +7443,22 @@
         <v>2019</v>
       </c>
       <c r="G54" s="79" t="s">
-        <v>297</v>
+        <v>304</v>
       </c>
       <c r="H54" s="29" t="s">
-        <v>298</v>
+        <v>271</v>
       </c>
       <c r="I54" s="56">
         <v>90</v>
       </c>
       <c r="J54" s="3" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="K54" s="10" t="s">
-        <v>299</v>
+        <v>272</v>
       </c>
       <c r="L54" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="M54" s="3">
         <v>1</v>
@@ -7473,7 +7470,7 @@
         <v>0</v>
       </c>
       <c r="P54" s="3" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="Q54" s="3">
         <v>0</v>
@@ -7489,13 +7486,13 @@
         <v>53</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>229</v>
+        <v>205</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="E55" s="3">
         <v>1</v>
@@ -7504,34 +7501,34 @@
         <v>2020</v>
       </c>
       <c r="G55" s="52" t="s">
-        <v>301</v>
+        <v>274</v>
       </c>
       <c r="H55" s="29" t="s">
-        <v>300</v>
+        <v>273</v>
       </c>
       <c r="I55" s="56">
         <v>10</v>
       </c>
       <c r="J55" s="3" t="s">
-        <v>257</v>
+        <v>231</v>
       </c>
       <c r="K55" s="4" t="s">
-        <v>303</v>
+        <v>276</v>
       </c>
       <c r="L55" s="3" t="s">
-        <v>271</v>
+        <v>245</v>
       </c>
       <c r="M55" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="N55" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="O55" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="P55" s="3" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="Q55" s="3">
         <v>1</v>
@@ -7875,7 +7872,7 @@
   <sheetData>
     <row r="1" spans="1:17">
       <c r="A1" s="60" t="s">
-        <v>260</v>
+        <v>234</v>
       </c>
       <c r="B1" s="66">
         <v>1</v>
@@ -7899,7 +7896,7 @@
         <v>7</v>
       </c>
       <c r="J1" s="60" t="s">
-        <v>260</v>
+        <v>234</v>
       </c>
       <c r="K1" s="66">
         <v>1</v>
@@ -7955,25 +7952,25 @@
       </c>
       <c r="J2" s="63"/>
       <c r="K2" s="61" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="L2" s="61" t="s">
-        <v>261</v>
+        <v>235</v>
       </c>
       <c r="M2" s="61" t="s">
-        <v>262</v>
+        <v>236</v>
       </c>
       <c r="N2" s="61" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="O2" s="61" t="s">
         <v>3</v>
       </c>
       <c r="P2" s="61" t="s">
-        <v>266</v>
+        <v>240</v>
       </c>
       <c r="Q2" s="61" t="s">
-        <v>267</v>
+        <v>241</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -8008,25 +8005,25 @@
       </c>
       <c r="J3" s="63"/>
       <c r="K3" s="64" t="s">
-        <v>186</v>
+        <v>166</v>
       </c>
       <c r="L3" s="64" t="s">
-        <v>187</v>
+        <v>167</v>
       </c>
       <c r="M3" s="64" t="s">
-        <v>263</v>
+        <v>237</v>
       </c>
       <c r="N3" s="64" t="s">
-        <v>188</v>
+        <v>168</v>
       </c>
       <c r="O3" s="64" t="s">
         <v>4</v>
       </c>
       <c r="P3" s="64" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="Q3" s="64" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -8052,14 +8049,14 @@
       <c r="H4" s="61"/>
       <c r="J4" s="63"/>
       <c r="K4" s="61" t="s">
-        <v>244</v>
+        <v>218</v>
       </c>
       <c r="L4" s="61"/>
       <c r="M4" s="65" t="s">
-        <v>264</v>
+        <v>238</v>
       </c>
       <c r="N4" s="61" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="O4" s="61" t="s">
         <v>5</v>
@@ -8084,7 +8081,7 @@
       <c r="L5" s="64"/>
       <c r="M5" s="64"/>
       <c r="N5" s="64" t="s">
-        <v>265</v>
+        <v>239</v>
       </c>
       <c r="O5" s="64"/>
       <c r="P5" s="64"/>

</xml_diff>